<commit_message>
changed the bulk import functionality and added history tracking for file upload
</commit_message>
<xml_diff>
--- a/Error_File.xlsx
+++ b/Error_File.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Master" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Leads" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet state="visible" name="Master" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Leads" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr/>
-  <extLst>
-    <ext uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
-  </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="F3" authorId="0">
+      <text>
+        <t>Invalid GSTIN</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Products</t>
   </si>
@@ -25,113 +37,101 @@
     <t>GSTR</t>
   </si>
   <si>
-    <t xml:space="preserve">ITC Reconsilation</t>
+    <t>ITC Reconsilation</t>
   </si>
   <si>
-    <t xml:space="preserve">E Invoice</t>
+    <t>E Invoice</t>
   </si>
   <si>
-    <t xml:space="preserve">EWay Bill</t>
+    <t>EWay Bill</t>
   </si>
   <si>
     <t>LMS</t>
   </si>
   <si>
-    <t xml:space="preserve">Third Eye</t>
+    <t>Third Eye</t>
   </si>
   <si>
-    <t xml:space="preserve">Safe Sign</t>
+    <t>Safe Sign</t>
   </si>
   <si>
-    <t xml:space="preserve">Sr No</t>
+    <t>Sr No</t>
   </si>
   <si>
-    <t xml:space="preserve">First Name (M)</t>
+    <t>First Name (M)</t>
   </si>
   <si>
-    <t xml:space="preserve">Last Name (M)</t>
+    <t>Last Name (M)</t>
   </si>
   <si>
-    <t xml:space="preserve">Mobile Number (M)</t>
+    <t>Mobile Number (M)</t>
   </si>
   <si>
-    <t xml:space="preserve">Email (M)</t>
+    <t>Email (M)</t>
   </si>
   <si>
-    <t xml:space="preserve">GSTIN (M)</t>
+    <t>GSTIN (M)</t>
   </si>
   <si>
-    <t xml:space="preserve">Interested Modules (M)</t>
+    <t>Interested Modules (M)</t>
   </si>
   <si>
-    <t xml:space="preserve">Business Address (O)</t>
+    <t>Business Address (O)</t>
   </si>
   <si>
-    <t xml:space="preserve">Description (O)</t>
+    <t>Description (O)</t>
   </si>
   <si>
-    <t>Akshay</t>
+    <t>Prashant</t>
   </si>
   <si>
-    <t>jadhav</t>
+    <t>Gaikwad</t>
   </si>
   <si>
-    <t>akshay@gmail.com</t>
+    <t>prashant2002@gmail.com</t>
   </si>
   <si>
-    <t>S34V5GWM69DVTAJ</t>
+    <t>ABCDRTYUIOP3Q</t>
   </si>
   <si>
-    <t>Rohan</t>
+    <t>Delhi</t>
   </si>
   <si>
-    <t>rhote</t>
-  </si>
-  <si>
-    <t>rohan@gmail.com</t>
-  </si>
-  <si>
-    <t>ABCDJERTYUIOPDQ</t>
+    <t>contacted by mail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="0"/>
   <fonts count="7">
     <font>
-      <sz val="10.000000"/>
-      <color indexed="64"/>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.000000"/>
-      <color indexed="64"/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.000000"/>
-      <color indexed="65"/>
+      <sz val="12.0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.000000"/>
-      <color indexed="64"/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="12.000000"/>
+      <sz val="12.0"/>
       <color rgb="FF002662"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10.000000"/>
-      <color theme="10"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -139,13 +139,19 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="10.000000"/>
+      <main:color theme="1"/>
+      <main:name val="Arial"/>
+      <main:scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -177,48 +183,32 @@
         <bgColor rgb="FFCFE2F3"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
+    <fill xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:patternFill patternType="solid">
+        <main:fgColor indexed="10"/>
+      </main:patternFill>
     </fill>
   </fills>
   <borders count="4">
+    <border/>
     <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
       <bottom style="thin">
         <color rgb="FF9FC5E8"/>
       </bottom>
-      <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
@@ -233,350 +223,71 @@
       <bottom style="thin">
         <color rgb="FF9FC5E8"/>
       </bottom>
-      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="15">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf fontId="2" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf fontId="3" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="3" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf fontId="3" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="4" fillId="4" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf fontId="4" fillId="5" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf fontId="4" fillId="6" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -633,7 +344,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -659,7 +370,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill>
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -736,7 +447,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill>
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -766,23 +477,19 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <outlinePr applyStyles="0" summaryBelow="0" summaryRight="0" showOutlineSymbols="1"/>
-    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:A46"/>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.630000000000001" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="27.25"/>
   </cols>
@@ -942,34 +649,27 @@
       <c r="A46" s="6"/>
     </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <outlinePr applyStyles="0" summaryBelow="0" summaryRight="0" showOutlineSymbols="1"/>
-    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.630000000000001" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" customWidth="true" width="16.63"/>
     <col min="3" max="3" customWidth="true" width="19.38"/>
-    <col min="4" max="4" customWidth="true" width="24.421875"/>
+    <col min="4" max="4" customWidth="true" width="20.0"/>
     <col min="5" max="5" customWidth="true" width="16.0"/>
-    <col min="6" max="6" customWidth="true" width="18.57421875"/>
-    <col min="7" max="7" customWidth="true" width="33.7109375"/>
-    <col min="8" max="8" customWidth="true" width="26.421875"/>
+    <col min="7" max="7" customWidth="true" width="22.75"/>
+    <col min="8" max="8" customWidth="true" width="21.88"/>
     <col min="9" max="9" customWidth="true" width="24.5"/>
   </cols>
   <sheetData>
@@ -1014,8 +714,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0">
-        <v>1</v>
+      <c r="A3" t="n" s="0">
+        <v>4.0</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>17</v>
@@ -1023,3071 +723,3025 @@
       <c r="C3" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="D3" s="0">
-        <v>8308575626</v>
+      <c r="D3" t="n" s="0">
+        <v>7.809926725E9</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s" s="14">
         <v>20</v>
       </c>
-      <c r="G3" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0">
+      <c r="G3" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>17</v>
+      <c r="H3" t="s" s="0">
+        <v>21</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>18</v>
+      <c r="I3" t="s" s="0">
+        <v>22</v>
       </c>
-      <c r="D4" s="0">
-        <v>8308575626</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="13" t="s">
+    </row>
+    <row r="4">
+      <c r="G4" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="D5" s="0">
-        <v>7809356725</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>1</v>
-      </c>
+      <c r="G5" s="13"/>
     </row>
     <row r="6">
-      <c r="G6" s="16"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="7">
-      <c r="G7" s="16"/>
+      <c r="G7" s="13"/>
     </row>
     <row r="8">
-      <c r="G8" s="16"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9">
-      <c r="G9" s="16"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10">
-      <c r="G10" s="16"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11">
-      <c r="G11" s="16"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12">
-      <c r="G12" s="16"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13">
-      <c r="G13" s="16"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14">
-      <c r="G14" s="16"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15">
-      <c r="G15" s="16"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16">
-      <c r="G16" s="16"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17">
-      <c r="G17" s="16"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18">
-      <c r="G18" s="16"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19">
-      <c r="G19" s="16"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20">
-      <c r="G20" s="16"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21">
-      <c r="G21" s="16"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22">
-      <c r="G22" s="16"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23">
-      <c r="G23" s="16"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24">
-      <c r="G24" s="16"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25">
-      <c r="G25" s="16"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26">
-      <c r="G26" s="16"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27">
-      <c r="G27" s="16"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28">
-      <c r="G28" s="16"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29">
-      <c r="G29" s="16"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30">
-      <c r="G30" s="16"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31">
-      <c r="G31" s="16"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32">
-      <c r="G32" s="16"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33">
-      <c r="G33" s="16"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34">
-      <c r="G34" s="16"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35">
-      <c r="G35" s="16"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36">
-      <c r="G36" s="16"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37">
-      <c r="G37" s="16"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38">
-      <c r="G38" s="16"/>
+      <c r="G38" s="13"/>
     </row>
     <row r="39">
-      <c r="G39" s="16"/>
+      <c r="G39" s="13"/>
     </row>
     <row r="40">
-      <c r="G40" s="16"/>
+      <c r="G40" s="13"/>
     </row>
     <row r="41">
-      <c r="G41" s="16"/>
+      <c r="G41" s="13"/>
     </row>
     <row r="42">
-      <c r="G42" s="16"/>
+      <c r="G42" s="13"/>
     </row>
     <row r="43">
-      <c r="G43" s="16"/>
+      <c r="G43" s="13"/>
     </row>
     <row r="44">
-      <c r="G44" s="16"/>
+      <c r="G44" s="13"/>
     </row>
     <row r="45">
-      <c r="G45" s="16"/>
+      <c r="G45" s="13"/>
     </row>
     <row r="46">
-      <c r="G46" s="16"/>
+      <c r="G46" s="13"/>
     </row>
     <row r="47">
-      <c r="G47" s="16"/>
+      <c r="G47" s="13"/>
     </row>
     <row r="48">
-      <c r="G48" s="16"/>
+      <c r="G48" s="13"/>
     </row>
     <row r="49">
-      <c r="G49" s="16"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50">
-      <c r="G50" s="16"/>
+      <c r="G50" s="13"/>
     </row>
     <row r="51">
-      <c r="G51" s="16"/>
+      <c r="G51" s="13"/>
     </row>
     <row r="52">
-      <c r="G52" s="16"/>
+      <c r="G52" s="13"/>
     </row>
     <row r="53">
-      <c r="G53" s="16"/>
+      <c r="G53" s="13"/>
     </row>
     <row r="54">
-      <c r="G54" s="16"/>
+      <c r="G54" s="13"/>
     </row>
     <row r="55">
-      <c r="G55" s="16"/>
+      <c r="G55" s="13"/>
     </row>
     <row r="56">
-      <c r="G56" s="16"/>
+      <c r="G56" s="13"/>
     </row>
     <row r="57">
-      <c r="G57" s="16"/>
+      <c r="G57" s="13"/>
     </row>
     <row r="58">
-      <c r="G58" s="16"/>
+      <c r="G58" s="13"/>
     </row>
     <row r="59">
-      <c r="G59" s="16"/>
+      <c r="G59" s="13"/>
     </row>
     <row r="60">
-      <c r="G60" s="16"/>
+      <c r="G60" s="13"/>
     </row>
     <row r="61">
-      <c r="G61" s="16"/>
+      <c r="G61" s="13"/>
     </row>
     <row r="62">
-      <c r="G62" s="16"/>
+      <c r="G62" s="13"/>
     </row>
     <row r="63">
-      <c r="G63" s="16"/>
+      <c r="G63" s="13"/>
     </row>
     <row r="64">
-      <c r="G64" s="16"/>
+      <c r="G64" s="13"/>
     </row>
     <row r="65">
-      <c r="G65" s="16"/>
+      <c r="G65" s="13"/>
     </row>
     <row r="66">
-      <c r="G66" s="16"/>
+      <c r="G66" s="13"/>
     </row>
     <row r="67">
-      <c r="G67" s="16"/>
+      <c r="G67" s="13"/>
     </row>
     <row r="68">
-      <c r="G68" s="16"/>
+      <c r="G68" s="13"/>
     </row>
     <row r="69">
-      <c r="G69" s="16"/>
+      <c r="G69" s="13"/>
     </row>
     <row r="70">
-      <c r="G70" s="16"/>
+      <c r="G70" s="13"/>
     </row>
     <row r="71">
-      <c r="G71" s="16"/>
+      <c r="G71" s="13"/>
     </row>
     <row r="72">
-      <c r="G72" s="16"/>
+      <c r="G72" s="13"/>
     </row>
     <row r="73">
-      <c r="G73" s="16"/>
+      <c r="G73" s="13"/>
     </row>
     <row r="74">
-      <c r="G74" s="16"/>
+      <c r="G74" s="13"/>
     </row>
     <row r="75">
-      <c r="G75" s="16"/>
+      <c r="G75" s="13"/>
     </row>
     <row r="76">
-      <c r="G76" s="16"/>
+      <c r="G76" s="13"/>
     </row>
     <row r="77">
-      <c r="G77" s="16"/>
+      <c r="G77" s="13"/>
     </row>
     <row r="78">
-      <c r="G78" s="16"/>
+      <c r="G78" s="13"/>
     </row>
     <row r="79">
-      <c r="G79" s="16"/>
+      <c r="G79" s="13"/>
     </row>
     <row r="80">
-      <c r="G80" s="16"/>
+      <c r="G80" s="13"/>
     </row>
     <row r="81">
-      <c r="G81" s="16"/>
+      <c r="G81" s="13"/>
     </row>
     <row r="82">
-      <c r="G82" s="16"/>
+      <c r="G82" s="13"/>
     </row>
     <row r="83">
-      <c r="G83" s="16"/>
+      <c r="G83" s="13"/>
     </row>
     <row r="84">
-      <c r="G84" s="16"/>
+      <c r="G84" s="13"/>
     </row>
     <row r="85">
-      <c r="G85" s="16"/>
+      <c r="G85" s="13"/>
     </row>
     <row r="86">
-      <c r="G86" s="16"/>
+      <c r="G86" s="13"/>
     </row>
     <row r="87">
-      <c r="G87" s="16"/>
+      <c r="G87" s="13"/>
     </row>
     <row r="88">
-      <c r="G88" s="16"/>
+      <c r="G88" s="13"/>
     </row>
     <row r="89">
-      <c r="G89" s="16"/>
+      <c r="G89" s="13"/>
     </row>
     <row r="90">
-      <c r="G90" s="16"/>
+      <c r="G90" s="13"/>
     </row>
     <row r="91">
-      <c r="G91" s="16"/>
+      <c r="G91" s="13"/>
     </row>
     <row r="92">
-      <c r="G92" s="16"/>
+      <c r="G92" s="13"/>
     </row>
     <row r="93">
-      <c r="G93" s="16"/>
+      <c r="G93" s="13"/>
     </row>
     <row r="94">
-      <c r="G94" s="16"/>
+      <c r="G94" s="13"/>
     </row>
     <row r="95">
-      <c r="G95" s="16"/>
+      <c r="G95" s="13"/>
     </row>
     <row r="96">
-      <c r="G96" s="16"/>
+      <c r="G96" s="13"/>
     </row>
     <row r="97">
-      <c r="G97" s="16"/>
+      <c r="G97" s="13"/>
     </row>
     <row r="98">
-      <c r="G98" s="16"/>
+      <c r="G98" s="13"/>
     </row>
     <row r="99">
-      <c r="G99" s="16"/>
+      <c r="G99" s="13"/>
     </row>
     <row r="100">
-      <c r="G100" s="16"/>
+      <c r="G100" s="13"/>
     </row>
     <row r="101">
-      <c r="G101" s="16"/>
+      <c r="G101" s="13"/>
     </row>
     <row r="102">
-      <c r="G102" s="16"/>
+      <c r="G102" s="13"/>
     </row>
     <row r="103">
-      <c r="G103" s="16"/>
+      <c r="G103" s="13"/>
     </row>
     <row r="104">
-      <c r="G104" s="16"/>
+      <c r="G104" s="13"/>
     </row>
     <row r="105">
-      <c r="G105" s="16"/>
+      <c r="G105" s="13"/>
     </row>
     <row r="106">
-      <c r="G106" s="16"/>
+      <c r="G106" s="13"/>
     </row>
     <row r="107">
-      <c r="G107" s="16"/>
+      <c r="G107" s="13"/>
     </row>
     <row r="108">
-      <c r="G108" s="16"/>
+      <c r="G108" s="13"/>
     </row>
     <row r="109">
-      <c r="G109" s="16"/>
+      <c r="G109" s="13"/>
     </row>
     <row r="110">
-      <c r="G110" s="16"/>
+      <c r="G110" s="13"/>
     </row>
     <row r="111">
-      <c r="G111" s="16"/>
+      <c r="G111" s="13"/>
     </row>
     <row r="112">
-      <c r="G112" s="16"/>
+      <c r="G112" s="13"/>
     </row>
     <row r="113">
-      <c r="G113" s="16"/>
+      <c r="G113" s="13"/>
     </row>
     <row r="114">
-      <c r="G114" s="16"/>
+      <c r="G114" s="13"/>
     </row>
     <row r="115">
-      <c r="G115" s="16"/>
+      <c r="G115" s="13"/>
     </row>
     <row r="116">
-      <c r="G116" s="16"/>
+      <c r="G116" s="13"/>
     </row>
     <row r="117">
-      <c r="G117" s="16"/>
+      <c r="G117" s="13"/>
     </row>
     <row r="118">
-      <c r="G118" s="16"/>
+      <c r="G118" s="13"/>
     </row>
     <row r="119">
-      <c r="G119" s="16"/>
+      <c r="G119" s="13"/>
     </row>
     <row r="120">
-      <c r="G120" s="16"/>
+      <c r="G120" s="13"/>
     </row>
     <row r="121">
-      <c r="G121" s="16"/>
+      <c r="G121" s="13"/>
     </row>
     <row r="122">
-      <c r="G122" s="16"/>
+      <c r="G122" s="13"/>
     </row>
     <row r="123">
-      <c r="G123" s="16"/>
+      <c r="G123" s="13"/>
     </row>
     <row r="124">
-      <c r="G124" s="16"/>
+      <c r="G124" s="13"/>
     </row>
     <row r="125">
-      <c r="G125" s="16"/>
+      <c r="G125" s="13"/>
     </row>
     <row r="126">
-      <c r="G126" s="16"/>
+      <c r="G126" s="13"/>
     </row>
     <row r="127">
-      <c r="G127" s="16"/>
+      <c r="G127" s="13"/>
     </row>
     <row r="128">
-      <c r="G128" s="16"/>
+      <c r="G128" s="13"/>
     </row>
     <row r="129">
-      <c r="G129" s="16"/>
+      <c r="G129" s="13"/>
     </row>
     <row r="130">
-      <c r="G130" s="16"/>
+      <c r="G130" s="13"/>
     </row>
     <row r="131">
-      <c r="G131" s="16"/>
+      <c r="G131" s="13"/>
     </row>
     <row r="132">
-      <c r="G132" s="16"/>
+      <c r="G132" s="13"/>
     </row>
     <row r="133">
-      <c r="G133" s="16"/>
+      <c r="G133" s="13"/>
     </row>
     <row r="134">
-      <c r="G134" s="16"/>
+      <c r="G134" s="13"/>
     </row>
     <row r="135">
-      <c r="G135" s="16"/>
+      <c r="G135" s="13"/>
     </row>
     <row r="136">
-      <c r="G136" s="16"/>
+      <c r="G136" s="13"/>
     </row>
     <row r="137">
-      <c r="G137" s="16"/>
+      <c r="G137" s="13"/>
     </row>
     <row r="138">
-      <c r="G138" s="16"/>
+      <c r="G138" s="13"/>
     </row>
     <row r="139">
-      <c r="G139" s="16"/>
+      <c r="G139" s="13"/>
     </row>
     <row r="140">
-      <c r="G140" s="16"/>
+      <c r="G140" s="13"/>
     </row>
     <row r="141">
-      <c r="G141" s="16"/>
+      <c r="G141" s="13"/>
     </row>
     <row r="142">
-      <c r="G142" s="16"/>
+      <c r="G142" s="13"/>
     </row>
     <row r="143">
-      <c r="G143" s="16"/>
+      <c r="G143" s="13"/>
     </row>
     <row r="144">
-      <c r="G144" s="16"/>
+      <c r="G144" s="13"/>
     </row>
     <row r="145">
-      <c r="G145" s="16"/>
+      <c r="G145" s="13"/>
     </row>
     <row r="146">
-      <c r="G146" s="16"/>
+      <c r="G146" s="13"/>
     </row>
     <row r="147">
-      <c r="G147" s="16"/>
+      <c r="G147" s="13"/>
     </row>
     <row r="148">
-      <c r="G148" s="16"/>
+      <c r="G148" s="13"/>
     </row>
     <row r="149">
-      <c r="G149" s="16"/>
+      <c r="G149" s="13"/>
     </row>
     <row r="150">
-      <c r="G150" s="16"/>
+      <c r="G150" s="13"/>
     </row>
     <row r="151">
-      <c r="G151" s="16"/>
+      <c r="G151" s="13"/>
     </row>
     <row r="152">
-      <c r="G152" s="16"/>
+      <c r="G152" s="13"/>
     </row>
     <row r="153">
-      <c r="G153" s="16"/>
+      <c r="G153" s="13"/>
     </row>
     <row r="154">
-      <c r="G154" s="16"/>
+      <c r="G154" s="13"/>
     </row>
     <row r="155">
-      <c r="G155" s="16"/>
+      <c r="G155" s="13"/>
     </row>
     <row r="156">
-      <c r="G156" s="16"/>
+      <c r="G156" s="13"/>
     </row>
     <row r="157">
-      <c r="G157" s="16"/>
+      <c r="G157" s="13"/>
     </row>
     <row r="158">
-      <c r="G158" s="16"/>
+      <c r="G158" s="13"/>
     </row>
     <row r="159">
-      <c r="G159" s="16"/>
+      <c r="G159" s="13"/>
     </row>
     <row r="160">
-      <c r="G160" s="16"/>
+      <c r="G160" s="13"/>
     </row>
     <row r="161">
-      <c r="G161" s="16"/>
+      <c r="G161" s="13"/>
     </row>
     <row r="162">
-      <c r="G162" s="16"/>
+      <c r="G162" s="13"/>
     </row>
     <row r="163">
-      <c r="G163" s="16"/>
+      <c r="G163" s="13"/>
     </row>
     <row r="164">
-      <c r="G164" s="16"/>
+      <c r="G164" s="13"/>
     </row>
     <row r="165">
-      <c r="G165" s="16"/>
+      <c r="G165" s="13"/>
     </row>
     <row r="166">
-      <c r="G166" s="16"/>
+      <c r="G166" s="13"/>
     </row>
     <row r="167">
-      <c r="G167" s="16"/>
+      <c r="G167" s="13"/>
     </row>
     <row r="168">
-      <c r="G168" s="16"/>
+      <c r="G168" s="13"/>
     </row>
     <row r="169">
-      <c r="G169" s="16"/>
+      <c r="G169" s="13"/>
     </row>
     <row r="170">
-      <c r="G170" s="16"/>
+      <c r="G170" s="13"/>
     </row>
     <row r="171">
-      <c r="G171" s="16"/>
+      <c r="G171" s="13"/>
     </row>
     <row r="172">
-      <c r="G172" s="16"/>
+      <c r="G172" s="13"/>
     </row>
     <row r="173">
-      <c r="G173" s="16"/>
+      <c r="G173" s="13"/>
     </row>
     <row r="174">
-      <c r="G174" s="16"/>
+      <c r="G174" s="13"/>
     </row>
     <row r="175">
-      <c r="G175" s="16"/>
+      <c r="G175" s="13"/>
     </row>
     <row r="176">
-      <c r="G176" s="16"/>
+      <c r="G176" s="13"/>
     </row>
     <row r="177">
-      <c r="G177" s="16"/>
+      <c r="G177" s="13"/>
     </row>
     <row r="178">
-      <c r="G178" s="16"/>
+      <c r="G178" s="13"/>
     </row>
     <row r="179">
-      <c r="G179" s="16"/>
+      <c r="G179" s="13"/>
     </row>
     <row r="180">
-      <c r="G180" s="16"/>
+      <c r="G180" s="13"/>
     </row>
     <row r="181">
-      <c r="G181" s="16"/>
+      <c r="G181" s="13"/>
     </row>
     <row r="182">
-      <c r="G182" s="16"/>
+      <c r="G182" s="13"/>
     </row>
     <row r="183">
-      <c r="G183" s="16"/>
+      <c r="G183" s="13"/>
     </row>
     <row r="184">
-      <c r="G184" s="16"/>
+      <c r="G184" s="13"/>
     </row>
     <row r="185">
-      <c r="G185" s="16"/>
+      <c r="G185" s="13"/>
     </row>
     <row r="186">
-      <c r="G186" s="16"/>
+      <c r="G186" s="13"/>
     </row>
     <row r="187">
-      <c r="G187" s="16"/>
+      <c r="G187" s="13"/>
     </row>
     <row r="188">
-      <c r="G188" s="16"/>
+      <c r="G188" s="13"/>
     </row>
     <row r="189">
-      <c r="G189" s="16"/>
+      <c r="G189" s="13"/>
     </row>
     <row r="190">
-      <c r="G190" s="16"/>
+      <c r="G190" s="13"/>
     </row>
     <row r="191">
-      <c r="G191" s="16"/>
+      <c r="G191" s="13"/>
     </row>
     <row r="192">
-      <c r="G192" s="16"/>
+      <c r="G192" s="13"/>
     </row>
     <row r="193">
-      <c r="G193" s="16"/>
+      <c r="G193" s="13"/>
     </row>
     <row r="194">
-      <c r="G194" s="16"/>
+      <c r="G194" s="13"/>
     </row>
     <row r="195">
-      <c r="G195" s="16"/>
+      <c r="G195" s="13"/>
     </row>
     <row r="196">
-      <c r="G196" s="16"/>
+      <c r="G196" s="13"/>
     </row>
     <row r="197">
-      <c r="G197" s="16"/>
+      <c r="G197" s="13"/>
     </row>
     <row r="198">
-      <c r="G198" s="16"/>
+      <c r="G198" s="13"/>
     </row>
     <row r="199">
-      <c r="G199" s="16"/>
+      <c r="G199" s="13"/>
     </row>
     <row r="200">
-      <c r="G200" s="16"/>
+      <c r="G200" s="13"/>
     </row>
     <row r="201">
-      <c r="G201" s="16"/>
+      <c r="G201" s="13"/>
     </row>
     <row r="202">
-      <c r="G202" s="16"/>
+      <c r="G202" s="13"/>
     </row>
     <row r="203">
-      <c r="G203" s="16"/>
+      <c r="G203" s="13"/>
     </row>
     <row r="204">
-      <c r="G204" s="16"/>
+      <c r="G204" s="13"/>
     </row>
     <row r="205">
-      <c r="G205" s="16"/>
+      <c r="G205" s="13"/>
     </row>
     <row r="206">
-      <c r="G206" s="16"/>
+      <c r="G206" s="13"/>
     </row>
     <row r="207">
-      <c r="G207" s="16"/>
+      <c r="G207" s="13"/>
     </row>
     <row r="208">
-      <c r="G208" s="16"/>
+      <c r="G208" s="13"/>
     </row>
     <row r="209">
-      <c r="G209" s="16"/>
+      <c r="G209" s="13"/>
     </row>
     <row r="210">
-      <c r="G210" s="16"/>
+      <c r="G210" s="13"/>
     </row>
     <row r="211">
-      <c r="G211" s="16"/>
+      <c r="G211" s="13"/>
     </row>
     <row r="212">
-      <c r="G212" s="16"/>
+      <c r="G212" s="13"/>
     </row>
     <row r="213">
-      <c r="G213" s="16"/>
+      <c r="G213" s="13"/>
     </row>
     <row r="214">
-      <c r="G214" s="16"/>
+      <c r="G214" s="13"/>
     </row>
     <row r="215">
-      <c r="G215" s="16"/>
+      <c r="G215" s="13"/>
     </row>
     <row r="216">
-      <c r="G216" s="16"/>
+      <c r="G216" s="13"/>
     </row>
     <row r="217">
-      <c r="G217" s="16"/>
+      <c r="G217" s="13"/>
     </row>
     <row r="218">
-      <c r="G218" s="16"/>
+      <c r="G218" s="13"/>
     </row>
     <row r="219">
-      <c r="G219" s="16"/>
+      <c r="G219" s="13"/>
     </row>
     <row r="220">
-      <c r="G220" s="16"/>
+      <c r="G220" s="13"/>
     </row>
     <row r="221">
-      <c r="G221" s="16"/>
+      <c r="G221" s="13"/>
     </row>
     <row r="222">
-      <c r="G222" s="16"/>
+      <c r="G222" s="13"/>
     </row>
     <row r="223">
-      <c r="G223" s="16"/>
+      <c r="G223" s="13"/>
     </row>
     <row r="224">
-      <c r="G224" s="16"/>
+      <c r="G224" s="13"/>
     </row>
     <row r="225">
-      <c r="G225" s="16"/>
+      <c r="G225" s="13"/>
     </row>
     <row r="226">
-      <c r="G226" s="16"/>
+      <c r="G226" s="13"/>
     </row>
     <row r="227">
-      <c r="G227" s="16"/>
+      <c r="G227" s="13"/>
     </row>
     <row r="228">
-      <c r="G228" s="16"/>
+      <c r="G228" s="13"/>
     </row>
     <row r="229">
-      <c r="G229" s="16"/>
+      <c r="G229" s="13"/>
     </row>
     <row r="230">
-      <c r="G230" s="16"/>
+      <c r="G230" s="13"/>
     </row>
     <row r="231">
-      <c r="G231" s="16"/>
+      <c r="G231" s="13"/>
     </row>
     <row r="232">
-      <c r="G232" s="16"/>
+      <c r="G232" s="13"/>
     </row>
     <row r="233">
-      <c r="G233" s="16"/>
+      <c r="G233" s="13"/>
     </row>
     <row r="234">
-      <c r="G234" s="16"/>
+      <c r="G234" s="13"/>
     </row>
     <row r="235">
-      <c r="G235" s="16"/>
+      <c r="G235" s="13"/>
     </row>
     <row r="236">
-      <c r="G236" s="16"/>
+      <c r="G236" s="13"/>
     </row>
     <row r="237">
-      <c r="G237" s="16"/>
+      <c r="G237" s="13"/>
     </row>
     <row r="238">
-      <c r="G238" s="16"/>
+      <c r="G238" s="13"/>
     </row>
     <row r="239">
-      <c r="G239" s="16"/>
+      <c r="G239" s="13"/>
     </row>
     <row r="240">
-      <c r="G240" s="16"/>
+      <c r="G240" s="13"/>
     </row>
     <row r="241">
-      <c r="G241" s="16"/>
+      <c r="G241" s="13"/>
     </row>
     <row r="242">
-      <c r="G242" s="16"/>
+      <c r="G242" s="13"/>
     </row>
     <row r="243">
-      <c r="G243" s="16"/>
+      <c r="G243" s="13"/>
     </row>
     <row r="244">
-      <c r="G244" s="16"/>
+      <c r="G244" s="13"/>
     </row>
     <row r="245">
-      <c r="G245" s="16"/>
+      <c r="G245" s="13"/>
     </row>
     <row r="246">
-      <c r="G246" s="16"/>
+      <c r="G246" s="13"/>
     </row>
     <row r="247">
-      <c r="G247" s="16"/>
+      <c r="G247" s="13"/>
     </row>
     <row r="248">
-      <c r="G248" s="16"/>
+      <c r="G248" s="13"/>
     </row>
     <row r="249">
-      <c r="G249" s="16"/>
+      <c r="G249" s="13"/>
     </row>
     <row r="250">
-      <c r="G250" s="16"/>
+      <c r="G250" s="13"/>
     </row>
     <row r="251">
-      <c r="G251" s="16"/>
+      <c r="G251" s="13"/>
     </row>
     <row r="252">
-      <c r="G252" s="16"/>
+      <c r="G252" s="13"/>
     </row>
     <row r="253">
-      <c r="G253" s="16"/>
+      <c r="G253" s="13"/>
     </row>
     <row r="254">
-      <c r="G254" s="16"/>
+      <c r="G254" s="13"/>
     </row>
     <row r="255">
-      <c r="G255" s="16"/>
+      <c r="G255" s="13"/>
     </row>
     <row r="256">
-      <c r="G256" s="16"/>
+      <c r="G256" s="13"/>
     </row>
     <row r="257">
-      <c r="G257" s="16"/>
+      <c r="G257" s="13"/>
     </row>
     <row r="258">
-      <c r="G258" s="16"/>
+      <c r="G258" s="13"/>
     </row>
     <row r="259">
-      <c r="G259" s="16"/>
+      <c r="G259" s="13"/>
     </row>
     <row r="260">
-      <c r="G260" s="16"/>
+      <c r="G260" s="13"/>
     </row>
     <row r="261">
-      <c r="G261" s="16"/>
+      <c r="G261" s="13"/>
     </row>
     <row r="262">
-      <c r="G262" s="16"/>
+      <c r="G262" s="13"/>
     </row>
     <row r="263">
-      <c r="G263" s="16"/>
+      <c r="G263" s="13"/>
     </row>
     <row r="264">
-      <c r="G264" s="16"/>
+      <c r="G264" s="13"/>
     </row>
     <row r="265">
-      <c r="G265" s="16"/>
+      <c r="G265" s="13"/>
     </row>
     <row r="266">
-      <c r="G266" s="16"/>
+      <c r="G266" s="13"/>
     </row>
     <row r="267">
-      <c r="G267" s="16"/>
+      <c r="G267" s="13"/>
     </row>
     <row r="268">
-      <c r="G268" s="16"/>
+      <c r="G268" s="13"/>
     </row>
     <row r="269">
-      <c r="G269" s="16"/>
+      <c r="G269" s="13"/>
     </row>
     <row r="270">
-      <c r="G270" s="16"/>
+      <c r="G270" s="13"/>
     </row>
     <row r="271">
-      <c r="G271" s="16"/>
+      <c r="G271" s="13"/>
     </row>
     <row r="272">
-      <c r="G272" s="16"/>
+      <c r="G272" s="13"/>
     </row>
     <row r="273">
-      <c r="G273" s="16"/>
+      <c r="G273" s="13"/>
     </row>
     <row r="274">
-      <c r="G274" s="16"/>
+      <c r="G274" s="13"/>
     </row>
     <row r="275">
-      <c r="G275" s="16"/>
+      <c r="G275" s="13"/>
     </row>
     <row r="276">
-      <c r="G276" s="16"/>
+      <c r="G276" s="13"/>
     </row>
     <row r="277">
-      <c r="G277" s="16"/>
+      <c r="G277" s="13"/>
     </row>
     <row r="278">
-      <c r="G278" s="16"/>
+      <c r="G278" s="13"/>
     </row>
     <row r="279">
-      <c r="G279" s="16"/>
+      <c r="G279" s="13"/>
     </row>
     <row r="280">
-      <c r="G280" s="16"/>
+      <c r="G280" s="13"/>
     </row>
     <row r="281">
-      <c r="G281" s="16"/>
+      <c r="G281" s="13"/>
     </row>
     <row r="282">
-      <c r="G282" s="16"/>
+      <c r="G282" s="13"/>
     </row>
     <row r="283">
-      <c r="G283" s="16"/>
+      <c r="G283" s="13"/>
     </row>
     <row r="284">
-      <c r="G284" s="16"/>
+      <c r="G284" s="13"/>
     </row>
     <row r="285">
-      <c r="G285" s="16"/>
+      <c r="G285" s="13"/>
     </row>
     <row r="286">
-      <c r="G286" s="16"/>
+      <c r="G286" s="13"/>
     </row>
     <row r="287">
-      <c r="G287" s="16"/>
+      <c r="G287" s="13"/>
     </row>
     <row r="288">
-      <c r="G288" s="16"/>
+      <c r="G288" s="13"/>
     </row>
     <row r="289">
-      <c r="G289" s="16"/>
+      <c r="G289" s="13"/>
     </row>
     <row r="290">
-      <c r="G290" s="16"/>
+      <c r="G290" s="13"/>
     </row>
     <row r="291">
-      <c r="G291" s="16"/>
+      <c r="G291" s="13"/>
     </row>
     <row r="292">
-      <c r="G292" s="16"/>
+      <c r="G292" s="13"/>
     </row>
     <row r="293">
-      <c r="G293" s="16"/>
+      <c r="G293" s="13"/>
     </row>
     <row r="294">
-      <c r="G294" s="16"/>
+      <c r="G294" s="13"/>
     </row>
     <row r="295">
-      <c r="G295" s="16"/>
+      <c r="G295" s="13"/>
     </row>
     <row r="296">
-      <c r="G296" s="16"/>
+      <c r="G296" s="13"/>
     </row>
     <row r="297">
-      <c r="G297" s="16"/>
+      <c r="G297" s="13"/>
     </row>
     <row r="298">
-      <c r="G298" s="16"/>
+      <c r="G298" s="13"/>
     </row>
     <row r="299">
-      <c r="G299" s="16"/>
+      <c r="G299" s="13"/>
     </row>
     <row r="300">
-      <c r="G300" s="16"/>
+      <c r="G300" s="13"/>
     </row>
     <row r="301">
-      <c r="G301" s="16"/>
+      <c r="G301" s="13"/>
     </row>
     <row r="302">
-      <c r="G302" s="16"/>
+      <c r="G302" s="13"/>
     </row>
     <row r="303">
-      <c r="G303" s="16"/>
+      <c r="G303" s="13"/>
     </row>
     <row r="304">
-      <c r="G304" s="16"/>
+      <c r="G304" s="13"/>
     </row>
     <row r="305">
-      <c r="G305" s="16"/>
+      <c r="G305" s="13"/>
     </row>
     <row r="306">
-      <c r="G306" s="16"/>
+      <c r="G306" s="13"/>
     </row>
     <row r="307">
-      <c r="G307" s="16"/>
+      <c r="G307" s="13"/>
     </row>
     <row r="308">
-      <c r="G308" s="16"/>
+      <c r="G308" s="13"/>
     </row>
     <row r="309">
-      <c r="G309" s="16"/>
+      <c r="G309" s="13"/>
     </row>
     <row r="310">
-      <c r="G310" s="16"/>
+      <c r="G310" s="13"/>
     </row>
     <row r="311">
-      <c r="G311" s="16"/>
+      <c r="G311" s="13"/>
     </row>
     <row r="312">
-      <c r="G312" s="16"/>
+      <c r="G312" s="13"/>
     </row>
     <row r="313">
-      <c r="G313" s="16"/>
+      <c r="G313" s="13"/>
     </row>
     <row r="314">
-      <c r="G314" s="16"/>
+      <c r="G314" s="13"/>
     </row>
     <row r="315">
-      <c r="G315" s="16"/>
+      <c r="G315" s="13"/>
     </row>
     <row r="316">
-      <c r="G316" s="16"/>
+      <c r="G316" s="13"/>
     </row>
     <row r="317">
-      <c r="G317" s="16"/>
+      <c r="G317" s="13"/>
     </row>
     <row r="318">
-      <c r="G318" s="16"/>
+      <c r="G318" s="13"/>
     </row>
     <row r="319">
-      <c r="G319" s="16"/>
+      <c r="G319" s="13"/>
     </row>
     <row r="320">
-      <c r="G320" s="16"/>
+      <c r="G320" s="13"/>
     </row>
     <row r="321">
-      <c r="G321" s="16"/>
+      <c r="G321" s="13"/>
     </row>
     <row r="322">
-      <c r="G322" s="16"/>
+      <c r="G322" s="13"/>
     </row>
     <row r="323">
-      <c r="G323" s="16"/>
+      <c r="G323" s="13"/>
     </row>
     <row r="324">
-      <c r="G324" s="16"/>
+      <c r="G324" s="13"/>
     </row>
     <row r="325">
-      <c r="G325" s="16"/>
+      <c r="G325" s="13"/>
     </row>
     <row r="326">
-      <c r="G326" s="16"/>
+      <c r="G326" s="13"/>
     </row>
     <row r="327">
-      <c r="G327" s="16"/>
+      <c r="G327" s="13"/>
     </row>
     <row r="328">
-      <c r="G328" s="16"/>
+      <c r="G328" s="13"/>
     </row>
     <row r="329">
-      <c r="G329" s="16"/>
+      <c r="G329" s="13"/>
     </row>
     <row r="330">
-      <c r="G330" s="16"/>
+      <c r="G330" s="13"/>
     </row>
     <row r="331">
-      <c r="G331" s="16"/>
+      <c r="G331" s="13"/>
     </row>
     <row r="332">
-      <c r="G332" s="16"/>
+      <c r="G332" s="13"/>
     </row>
     <row r="333">
-      <c r="G333" s="16"/>
+      <c r="G333" s="13"/>
     </row>
     <row r="334">
-      <c r="G334" s="16"/>
+      <c r="G334" s="13"/>
     </row>
     <row r="335">
-      <c r="G335" s="16"/>
+      <c r="G335" s="13"/>
     </row>
     <row r="336">
-      <c r="G336" s="16"/>
+      <c r="G336" s="13"/>
     </row>
     <row r="337">
-      <c r="G337" s="16"/>
+      <c r="G337" s="13"/>
     </row>
     <row r="338">
-      <c r="G338" s="16"/>
+      <c r="G338" s="13"/>
     </row>
     <row r="339">
-      <c r="G339" s="16"/>
+      <c r="G339" s="13"/>
     </row>
     <row r="340">
-      <c r="G340" s="16"/>
+      <c r="G340" s="13"/>
     </row>
     <row r="341">
-      <c r="G341" s="16"/>
+      <c r="G341" s="13"/>
     </row>
     <row r="342">
-      <c r="G342" s="16"/>
+      <c r="G342" s="13"/>
     </row>
     <row r="343">
-      <c r="G343" s="16"/>
+      <c r="G343" s="13"/>
     </row>
     <row r="344">
-      <c r="G344" s="16"/>
+      <c r="G344" s="13"/>
     </row>
     <row r="345">
-      <c r="G345" s="16"/>
+      <c r="G345" s="13"/>
     </row>
     <row r="346">
-      <c r="G346" s="16"/>
+      <c r="G346" s="13"/>
     </row>
     <row r="347">
-      <c r="G347" s="16"/>
+      <c r="G347" s="13"/>
     </row>
     <row r="348">
-      <c r="G348" s="16"/>
+      <c r="G348" s="13"/>
     </row>
     <row r="349">
-      <c r="G349" s="16"/>
+      <c r="G349" s="13"/>
     </row>
     <row r="350">
-      <c r="G350" s="16"/>
+      <c r="G350" s="13"/>
     </row>
     <row r="351">
-      <c r="G351" s="16"/>
+      <c r="G351" s="13"/>
     </row>
     <row r="352">
-      <c r="G352" s="16"/>
+      <c r="G352" s="13"/>
     </row>
     <row r="353">
-      <c r="G353" s="16"/>
+      <c r="G353" s="13"/>
     </row>
     <row r="354">
-      <c r="G354" s="16"/>
+      <c r="G354" s="13"/>
     </row>
     <row r="355">
-      <c r="G355" s="16"/>
+      <c r="G355" s="13"/>
     </row>
     <row r="356">
-      <c r="G356" s="16"/>
+      <c r="G356" s="13"/>
     </row>
     <row r="357">
-      <c r="G357" s="16"/>
+      <c r="G357" s="13"/>
     </row>
     <row r="358">
-      <c r="G358" s="16"/>
+      <c r="G358" s="13"/>
     </row>
     <row r="359">
-      <c r="G359" s="16"/>
+      <c r="G359" s="13"/>
     </row>
     <row r="360">
-      <c r="G360" s="16"/>
+      <c r="G360" s="13"/>
     </row>
     <row r="361">
-      <c r="G361" s="16"/>
+      <c r="G361" s="13"/>
     </row>
     <row r="362">
-      <c r="G362" s="16"/>
+      <c r="G362" s="13"/>
     </row>
     <row r="363">
-      <c r="G363" s="16"/>
+      <c r="G363" s="13"/>
     </row>
     <row r="364">
-      <c r="G364" s="16"/>
+      <c r="G364" s="13"/>
     </row>
     <row r="365">
-      <c r="G365" s="16"/>
+      <c r="G365" s="13"/>
     </row>
     <row r="366">
-      <c r="G366" s="16"/>
+      <c r="G366" s="13"/>
     </row>
     <row r="367">
-      <c r="G367" s="16"/>
+      <c r="G367" s="13"/>
     </row>
     <row r="368">
-      <c r="G368" s="16"/>
+      <c r="G368" s="13"/>
     </row>
     <row r="369">
-      <c r="G369" s="16"/>
+      <c r="G369" s="13"/>
     </row>
     <row r="370">
-      <c r="G370" s="16"/>
+      <c r="G370" s="13"/>
     </row>
     <row r="371">
-      <c r="G371" s="16"/>
+      <c r="G371" s="13"/>
     </row>
     <row r="372">
-      <c r="G372" s="16"/>
+      <c r="G372" s="13"/>
     </row>
     <row r="373">
-      <c r="G373" s="16"/>
+      <c r="G373" s="13"/>
     </row>
     <row r="374">
-      <c r="G374" s="16"/>
+      <c r="G374" s="13"/>
     </row>
     <row r="375">
-      <c r="G375" s="16"/>
+      <c r="G375" s="13"/>
     </row>
     <row r="376">
-      <c r="G376" s="16"/>
+      <c r="G376" s="13"/>
     </row>
     <row r="377">
-      <c r="G377" s="16"/>
+      <c r="G377" s="13"/>
     </row>
     <row r="378">
-      <c r="G378" s="16"/>
+      <c r="G378" s="13"/>
     </row>
     <row r="379">
-      <c r="G379" s="16"/>
+      <c r="G379" s="13"/>
     </row>
     <row r="380">
-      <c r="G380" s="16"/>
+      <c r="G380" s="13"/>
     </row>
     <row r="381">
-      <c r="G381" s="16"/>
+      <c r="G381" s="13"/>
     </row>
     <row r="382">
-      <c r="G382" s="16"/>
+      <c r="G382" s="13"/>
     </row>
     <row r="383">
-      <c r="G383" s="16"/>
+      <c r="G383" s="13"/>
     </row>
     <row r="384">
-      <c r="G384" s="16"/>
+      <c r="G384" s="13"/>
     </row>
     <row r="385">
-      <c r="G385" s="16"/>
+      <c r="G385" s="13"/>
     </row>
     <row r="386">
-      <c r="G386" s="16"/>
+      <c r="G386" s="13"/>
     </row>
     <row r="387">
-      <c r="G387" s="16"/>
+      <c r="G387" s="13"/>
     </row>
     <row r="388">
-      <c r="G388" s="16"/>
+      <c r="G388" s="13"/>
     </row>
     <row r="389">
-      <c r="G389" s="16"/>
+      <c r="G389" s="13"/>
     </row>
     <row r="390">
-      <c r="G390" s="16"/>
+      <c r="G390" s="13"/>
     </row>
     <row r="391">
-      <c r="G391" s="16"/>
+      <c r="G391" s="13"/>
     </row>
     <row r="392">
-      <c r="G392" s="16"/>
+      <c r="G392" s="13"/>
     </row>
     <row r="393">
-      <c r="G393" s="16"/>
+      <c r="G393" s="13"/>
     </row>
     <row r="394">
-      <c r="G394" s="16"/>
+      <c r="G394" s="13"/>
     </row>
     <row r="395">
-      <c r="G395" s="16"/>
+      <c r="G395" s="13"/>
     </row>
     <row r="396">
-      <c r="G396" s="16"/>
+      <c r="G396" s="13"/>
     </row>
     <row r="397">
-      <c r="G397" s="16"/>
+      <c r="G397" s="13"/>
     </row>
     <row r="398">
-      <c r="G398" s="16"/>
+      <c r="G398" s="13"/>
     </row>
     <row r="399">
-      <c r="G399" s="16"/>
+      <c r="G399" s="13"/>
     </row>
     <row r="400">
-      <c r="G400" s="16"/>
+      <c r="G400" s="13"/>
     </row>
     <row r="401">
-      <c r="G401" s="16"/>
+      <c r="G401" s="13"/>
     </row>
     <row r="402">
-      <c r="G402" s="16"/>
+      <c r="G402" s="13"/>
     </row>
     <row r="403">
-      <c r="G403" s="16"/>
+      <c r="G403" s="13"/>
     </row>
     <row r="404">
-      <c r="G404" s="16"/>
+      <c r="G404" s="13"/>
     </row>
     <row r="405">
-      <c r="G405" s="16"/>
+      <c r="G405" s="13"/>
     </row>
     <row r="406">
-      <c r="G406" s="16"/>
+      <c r="G406" s="13"/>
     </row>
     <row r="407">
-      <c r="G407" s="16"/>
+      <c r="G407" s="13"/>
     </row>
     <row r="408">
-      <c r="G408" s="16"/>
+      <c r="G408" s="13"/>
     </row>
     <row r="409">
-      <c r="G409" s="16"/>
+      <c r="G409" s="13"/>
     </row>
     <row r="410">
-      <c r="G410" s="16"/>
+      <c r="G410" s="13"/>
     </row>
     <row r="411">
-      <c r="G411" s="16"/>
+      <c r="G411" s="13"/>
     </row>
     <row r="412">
-      <c r="G412" s="16"/>
+      <c r="G412" s="13"/>
     </row>
     <row r="413">
-      <c r="G413" s="16"/>
+      <c r="G413" s="13"/>
     </row>
     <row r="414">
-      <c r="G414" s="16"/>
+      <c r="G414" s="13"/>
     </row>
     <row r="415">
-      <c r="G415" s="16"/>
+      <c r="G415" s="13"/>
     </row>
     <row r="416">
-      <c r="G416" s="16"/>
+      <c r="G416" s="13"/>
     </row>
     <row r="417">
-      <c r="G417" s="16"/>
+      <c r="G417" s="13"/>
     </row>
     <row r="418">
-      <c r="G418" s="16"/>
+      <c r="G418" s="13"/>
     </row>
     <row r="419">
-      <c r="G419" s="16"/>
+      <c r="G419" s="13"/>
     </row>
     <row r="420">
-      <c r="G420" s="16"/>
+      <c r="G420" s="13"/>
     </row>
     <row r="421">
-      <c r="G421" s="16"/>
+      <c r="G421" s="13"/>
     </row>
     <row r="422">
-      <c r="G422" s="16"/>
+      <c r="G422" s="13"/>
     </row>
     <row r="423">
-      <c r="G423" s="16"/>
+      <c r="G423" s="13"/>
     </row>
     <row r="424">
-      <c r="G424" s="16"/>
+      <c r="G424" s="13"/>
     </row>
     <row r="425">
-      <c r="G425" s="16"/>
+      <c r="G425" s="13"/>
     </row>
     <row r="426">
-      <c r="G426" s="16"/>
+      <c r="G426" s="13"/>
     </row>
     <row r="427">
-      <c r="G427" s="16"/>
+      <c r="G427" s="13"/>
     </row>
     <row r="428">
-      <c r="G428" s="16"/>
+      <c r="G428" s="13"/>
     </row>
     <row r="429">
-      <c r="G429" s="16"/>
+      <c r="G429" s="13"/>
     </row>
     <row r="430">
-      <c r="G430" s="16"/>
+      <c r="G430" s="13"/>
     </row>
     <row r="431">
-      <c r="G431" s="16"/>
+      <c r="G431" s="13"/>
     </row>
     <row r="432">
-      <c r="G432" s="16"/>
+      <c r="G432" s="13"/>
     </row>
     <row r="433">
-      <c r="G433" s="16"/>
+      <c r="G433" s="13"/>
     </row>
     <row r="434">
-      <c r="G434" s="16"/>
+      <c r="G434" s="13"/>
     </row>
     <row r="435">
-      <c r="G435" s="16"/>
+      <c r="G435" s="13"/>
     </row>
     <row r="436">
-      <c r="G436" s="16"/>
+      <c r="G436" s="13"/>
     </row>
     <row r="437">
-      <c r="G437" s="16"/>
+      <c r="G437" s="13"/>
     </row>
     <row r="438">
-      <c r="G438" s="16"/>
+      <c r="G438" s="13"/>
     </row>
     <row r="439">
-      <c r="G439" s="16"/>
+      <c r="G439" s="13"/>
     </row>
     <row r="440">
-      <c r="G440" s="16"/>
+      <c r="G440" s="13"/>
     </row>
     <row r="441">
-      <c r="G441" s="16"/>
+      <c r="G441" s="13"/>
     </row>
     <row r="442">
-      <c r="G442" s="16"/>
+      <c r="G442" s="13"/>
     </row>
     <row r="443">
-      <c r="G443" s="16"/>
+      <c r="G443" s="13"/>
     </row>
     <row r="444">
-      <c r="G444" s="16"/>
+      <c r="G444" s="13"/>
     </row>
     <row r="445">
-      <c r="G445" s="16"/>
+      <c r="G445" s="13"/>
     </row>
     <row r="446">
-      <c r="G446" s="16"/>
+      <c r="G446" s="13"/>
     </row>
     <row r="447">
-      <c r="G447" s="16"/>
+      <c r="G447" s="13"/>
     </row>
     <row r="448">
-      <c r="G448" s="16"/>
+      <c r="G448" s="13"/>
     </row>
     <row r="449">
-      <c r="G449" s="16"/>
+      <c r="G449" s="13"/>
     </row>
     <row r="450">
-      <c r="G450" s="16"/>
+      <c r="G450" s="13"/>
     </row>
     <row r="451">
-      <c r="G451" s="16"/>
+      <c r="G451" s="13"/>
     </row>
     <row r="452">
-      <c r="G452" s="16"/>
+      <c r="G452" s="13"/>
     </row>
     <row r="453">
-      <c r="G453" s="16"/>
+      <c r="G453" s="13"/>
     </row>
     <row r="454">
-      <c r="G454" s="16"/>
+      <c r="G454" s="13"/>
     </row>
     <row r="455">
-      <c r="G455" s="16"/>
+      <c r="G455" s="13"/>
     </row>
     <row r="456">
-      <c r="G456" s="16"/>
+      <c r="G456" s="13"/>
     </row>
     <row r="457">
-      <c r="G457" s="16"/>
+      <c r="G457" s="13"/>
     </row>
     <row r="458">
-      <c r="G458" s="16"/>
+      <c r="G458" s="13"/>
     </row>
     <row r="459">
-      <c r="G459" s="16"/>
+      <c r="G459" s="13"/>
     </row>
     <row r="460">
-      <c r="G460" s="16"/>
+      <c r="G460" s="13"/>
     </row>
     <row r="461">
-      <c r="G461" s="16"/>
+      <c r="G461" s="13"/>
     </row>
     <row r="462">
-      <c r="G462" s="16"/>
+      <c r="G462" s="13"/>
     </row>
     <row r="463">
-      <c r="G463" s="16"/>
+      <c r="G463" s="13"/>
     </row>
     <row r="464">
-      <c r="G464" s="16"/>
+      <c r="G464" s="13"/>
     </row>
     <row r="465">
-      <c r="G465" s="16"/>
+      <c r="G465" s="13"/>
     </row>
     <row r="466">
-      <c r="G466" s="16"/>
+      <c r="G466" s="13"/>
     </row>
     <row r="467">
-      <c r="G467" s="16"/>
+      <c r="G467" s="13"/>
     </row>
     <row r="468">
-      <c r="G468" s="16"/>
+      <c r="G468" s="13"/>
     </row>
     <row r="469">
-      <c r="G469" s="16"/>
+      <c r="G469" s="13"/>
     </row>
     <row r="470">
-      <c r="G470" s="16"/>
+      <c r="G470" s="13"/>
     </row>
     <row r="471">
-      <c r="G471" s="16"/>
+      <c r="G471" s="13"/>
     </row>
     <row r="472">
-      <c r="G472" s="16"/>
+      <c r="G472" s="13"/>
     </row>
     <row r="473">
-      <c r="G473" s="16"/>
+      <c r="G473" s="13"/>
     </row>
     <row r="474">
-      <c r="G474" s="16"/>
+      <c r="G474" s="13"/>
     </row>
     <row r="475">
-      <c r="G475" s="16"/>
+      <c r="G475" s="13"/>
     </row>
     <row r="476">
-      <c r="G476" s="16"/>
+      <c r="G476" s="13"/>
     </row>
     <row r="477">
-      <c r="G477" s="16"/>
+      <c r="G477" s="13"/>
     </row>
     <row r="478">
-      <c r="G478" s="16"/>
+      <c r="G478" s="13"/>
     </row>
     <row r="479">
-      <c r="G479" s="16"/>
+      <c r="G479" s="13"/>
     </row>
     <row r="480">
-      <c r="G480" s="16"/>
+      <c r="G480" s="13"/>
     </row>
     <row r="481">
-      <c r="G481" s="16"/>
+      <c r="G481" s="13"/>
     </row>
     <row r="482">
-      <c r="G482" s="16"/>
+      <c r="G482" s="13"/>
     </row>
     <row r="483">
-      <c r="G483" s="16"/>
+      <c r="G483" s="13"/>
     </row>
     <row r="484">
-      <c r="G484" s="16"/>
+      <c r="G484" s="13"/>
     </row>
     <row r="485">
-      <c r="G485" s="16"/>
+      <c r="G485" s="13"/>
     </row>
     <row r="486">
-      <c r="G486" s="16"/>
+      <c r="G486" s="13"/>
     </row>
     <row r="487">
-      <c r="G487" s="16"/>
+      <c r="G487" s="13"/>
     </row>
     <row r="488">
-      <c r="G488" s="16"/>
+      <c r="G488" s="13"/>
     </row>
     <row r="489">
-      <c r="G489" s="16"/>
+      <c r="G489" s="13"/>
     </row>
     <row r="490">
-      <c r="G490" s="16"/>
+      <c r="G490" s="13"/>
     </row>
     <row r="491">
-      <c r="G491" s="16"/>
+      <c r="G491" s="13"/>
     </row>
     <row r="492">
-      <c r="G492" s="16"/>
+      <c r="G492" s="13"/>
     </row>
     <row r="493">
-      <c r="G493" s="16"/>
+      <c r="G493" s="13"/>
     </row>
     <row r="494">
-      <c r="G494" s="16"/>
+      <c r="G494" s="13"/>
     </row>
     <row r="495">
-      <c r="G495" s="16"/>
+      <c r="G495" s="13"/>
     </row>
     <row r="496">
-      <c r="G496" s="16"/>
+      <c r="G496" s="13"/>
     </row>
     <row r="497">
-      <c r="G497" s="16"/>
+      <c r="G497" s="13"/>
     </row>
     <row r="498">
-      <c r="G498" s="16"/>
+      <c r="G498" s="13"/>
     </row>
     <row r="499">
-      <c r="G499" s="16"/>
+      <c r="G499" s="13"/>
     </row>
     <row r="500">
-      <c r="G500" s="16"/>
+      <c r="G500" s="13"/>
     </row>
     <row r="501">
-      <c r="G501" s="16"/>
+      <c r="G501" s="13"/>
     </row>
     <row r="502">
-      <c r="G502" s="16"/>
+      <c r="G502" s="13"/>
     </row>
     <row r="503">
-      <c r="G503" s="16"/>
+      <c r="G503" s="13"/>
     </row>
     <row r="504">
-      <c r="G504" s="16"/>
+      <c r="G504" s="13"/>
     </row>
     <row r="505">
-      <c r="G505" s="16"/>
+      <c r="G505" s="13"/>
     </row>
     <row r="506">
-      <c r="G506" s="16"/>
+      <c r="G506" s="13"/>
     </row>
     <row r="507">
-      <c r="G507" s="16"/>
+      <c r="G507" s="13"/>
     </row>
     <row r="508">
-      <c r="G508" s="16"/>
+      <c r="G508" s="13"/>
     </row>
     <row r="509">
-      <c r="G509" s="16"/>
+      <c r="G509" s="13"/>
     </row>
     <row r="510">
-      <c r="G510" s="16"/>
+      <c r="G510" s="13"/>
     </row>
     <row r="511">
-      <c r="G511" s="16"/>
+      <c r="G511" s="13"/>
     </row>
     <row r="512">
-      <c r="G512" s="16"/>
+      <c r="G512" s="13"/>
     </row>
     <row r="513">
-      <c r="G513" s="16"/>
+      <c r="G513" s="13"/>
     </row>
     <row r="514">
-      <c r="G514" s="16"/>
+      <c r="G514" s="13"/>
     </row>
     <row r="515">
-      <c r="G515" s="16"/>
+      <c r="G515" s="13"/>
     </row>
     <row r="516">
-      <c r="G516" s="16"/>
+      <c r="G516" s="13"/>
     </row>
     <row r="517">
-      <c r="G517" s="16"/>
+      <c r="G517" s="13"/>
     </row>
     <row r="518">
-      <c r="G518" s="16"/>
+      <c r="G518" s="13"/>
     </row>
     <row r="519">
-      <c r="G519" s="16"/>
+      <c r="G519" s="13"/>
     </row>
     <row r="520">
-      <c r="G520" s="16"/>
+      <c r="G520" s="13"/>
     </row>
     <row r="521">
-      <c r="G521" s="16"/>
+      <c r="G521" s="13"/>
     </row>
     <row r="522">
-      <c r="G522" s="16"/>
+      <c r="G522" s="13"/>
     </row>
     <row r="523">
-      <c r="G523" s="16"/>
+      <c r="G523" s="13"/>
     </row>
     <row r="524">
-      <c r="G524" s="16"/>
+      <c r="G524" s="13"/>
     </row>
     <row r="525">
-      <c r="G525" s="16"/>
+      <c r="G525" s="13"/>
     </row>
     <row r="526">
-      <c r="G526" s="16"/>
+      <c r="G526" s="13"/>
     </row>
     <row r="527">
-      <c r="G527" s="16"/>
+      <c r="G527" s="13"/>
     </row>
     <row r="528">
-      <c r="G528" s="16"/>
+      <c r="G528" s="13"/>
     </row>
     <row r="529">
-      <c r="G529" s="16"/>
+      <c r="G529" s="13"/>
     </row>
     <row r="530">
-      <c r="G530" s="16"/>
+      <c r="G530" s="13"/>
     </row>
     <row r="531">
-      <c r="G531" s="16"/>
+      <c r="G531" s="13"/>
     </row>
     <row r="532">
-      <c r="G532" s="16"/>
+      <c r="G532" s="13"/>
     </row>
     <row r="533">
-      <c r="G533" s="16"/>
+      <c r="G533" s="13"/>
     </row>
     <row r="534">
-      <c r="G534" s="16"/>
+      <c r="G534" s="13"/>
     </row>
     <row r="535">
-      <c r="G535" s="16"/>
+      <c r="G535" s="13"/>
     </row>
     <row r="536">
-      <c r="G536" s="16"/>
+      <c r="G536" s="13"/>
     </row>
     <row r="537">
-      <c r="G537" s="16"/>
+      <c r="G537" s="13"/>
     </row>
     <row r="538">
-      <c r="G538" s="16"/>
+      <c r="G538" s="13"/>
     </row>
     <row r="539">
-      <c r="G539" s="16"/>
+      <c r="G539" s="13"/>
     </row>
     <row r="540">
-      <c r="G540" s="16"/>
+      <c r="G540" s="13"/>
     </row>
     <row r="541">
-      <c r="G541" s="16"/>
+      <c r="G541" s="13"/>
     </row>
     <row r="542">
-      <c r="G542" s="16"/>
+      <c r="G542" s="13"/>
     </row>
     <row r="543">
-      <c r="G543" s="16"/>
+      <c r="G543" s="13"/>
     </row>
     <row r="544">
-      <c r="G544" s="16"/>
+      <c r="G544" s="13"/>
     </row>
     <row r="545">
-      <c r="G545" s="16"/>
+      <c r="G545" s="13"/>
     </row>
     <row r="546">
-      <c r="G546" s="16"/>
+      <c r="G546" s="13"/>
     </row>
     <row r="547">
-      <c r="G547" s="16"/>
+      <c r="G547" s="13"/>
     </row>
     <row r="548">
-      <c r="G548" s="16"/>
+      <c r="G548" s="13"/>
     </row>
     <row r="549">
-      <c r="G549" s="16"/>
+      <c r="G549" s="13"/>
     </row>
     <row r="550">
-      <c r="G550" s="16"/>
+      <c r="G550" s="13"/>
     </row>
     <row r="551">
-      <c r="G551" s="16"/>
+      <c r="G551" s="13"/>
     </row>
     <row r="552">
-      <c r="G552" s="16"/>
+      <c r="G552" s="13"/>
     </row>
     <row r="553">
-      <c r="G553" s="16"/>
+      <c r="G553" s="13"/>
     </row>
     <row r="554">
-      <c r="G554" s="16"/>
+      <c r="G554" s="13"/>
     </row>
     <row r="555">
-      <c r="G555" s="16"/>
+      <c r="G555" s="13"/>
     </row>
     <row r="556">
-      <c r="G556" s="16"/>
+      <c r="G556" s="13"/>
     </row>
     <row r="557">
-      <c r="G557" s="16"/>
+      <c r="G557" s="13"/>
     </row>
     <row r="558">
-      <c r="G558" s="16"/>
+      <c r="G558" s="13"/>
     </row>
     <row r="559">
-      <c r="G559" s="16"/>
+      <c r="G559" s="13"/>
     </row>
     <row r="560">
-      <c r="G560" s="16"/>
+      <c r="G560" s="13"/>
     </row>
     <row r="561">
-      <c r="G561" s="16"/>
+      <c r="G561" s="13"/>
     </row>
     <row r="562">
-      <c r="G562" s="16"/>
+      <c r="G562" s="13"/>
     </row>
     <row r="563">
-      <c r="G563" s="16"/>
+      <c r="G563" s="13"/>
     </row>
     <row r="564">
-      <c r="G564" s="16"/>
+      <c r="G564" s="13"/>
     </row>
     <row r="565">
-      <c r="G565" s="16"/>
+      <c r="G565" s="13"/>
     </row>
     <row r="566">
-      <c r="G566" s="16"/>
+      <c r="G566" s="13"/>
     </row>
     <row r="567">
-      <c r="G567" s="16"/>
+      <c r="G567" s="13"/>
     </row>
     <row r="568">
-      <c r="G568" s="16"/>
+      <c r="G568" s="13"/>
     </row>
     <row r="569">
-      <c r="G569" s="16"/>
+      <c r="G569" s="13"/>
     </row>
     <row r="570">
-      <c r="G570" s="16"/>
+      <c r="G570" s="13"/>
     </row>
     <row r="571">
-      <c r="G571" s="16"/>
+      <c r="G571" s="13"/>
     </row>
     <row r="572">
-      <c r="G572" s="16"/>
+      <c r="G572" s="13"/>
     </row>
     <row r="573">
-      <c r="G573" s="16"/>
+      <c r="G573" s="13"/>
     </row>
     <row r="574">
-      <c r="G574" s="16"/>
+      <c r="G574" s="13"/>
     </row>
     <row r="575">
-      <c r="G575" s="16"/>
+      <c r="G575" s="13"/>
     </row>
     <row r="576">
-      <c r="G576" s="16"/>
+      <c r="G576" s="13"/>
     </row>
     <row r="577">
-      <c r="G577" s="16"/>
+      <c r="G577" s="13"/>
     </row>
     <row r="578">
-      <c r="G578" s="16"/>
+      <c r="G578" s="13"/>
     </row>
     <row r="579">
-      <c r="G579" s="16"/>
+      <c r="G579" s="13"/>
     </row>
     <row r="580">
-      <c r="G580" s="16"/>
+      <c r="G580" s="13"/>
     </row>
     <row r="581">
-      <c r="G581" s="16"/>
+      <c r="G581" s="13"/>
     </row>
     <row r="582">
-      <c r="G582" s="16"/>
+      <c r="G582" s="13"/>
     </row>
     <row r="583">
-      <c r="G583" s="16"/>
+      <c r="G583" s="13"/>
     </row>
     <row r="584">
-      <c r="G584" s="16"/>
+      <c r="G584" s="13"/>
     </row>
     <row r="585">
-      <c r="G585" s="16"/>
+      <c r="G585" s="13"/>
     </row>
     <row r="586">
-      <c r="G586" s="16"/>
+      <c r="G586" s="13"/>
     </row>
     <row r="587">
-      <c r="G587" s="16"/>
+      <c r="G587" s="13"/>
     </row>
     <row r="588">
-      <c r="G588" s="16"/>
+      <c r="G588" s="13"/>
     </row>
     <row r="589">
-      <c r="G589" s="16"/>
+      <c r="G589" s="13"/>
     </row>
     <row r="590">
-      <c r="G590" s="16"/>
+      <c r="G590" s="13"/>
     </row>
     <row r="591">
-      <c r="G591" s="16"/>
+      <c r="G591" s="13"/>
     </row>
     <row r="592">
-      <c r="G592" s="16"/>
+      <c r="G592" s="13"/>
     </row>
     <row r="593">
-      <c r="G593" s="16"/>
+      <c r="G593" s="13"/>
     </row>
     <row r="594">
-      <c r="G594" s="16"/>
+      <c r="G594" s="13"/>
     </row>
     <row r="595">
-      <c r="G595" s="16"/>
+      <c r="G595" s="13"/>
     </row>
     <row r="596">
-      <c r="G596" s="16"/>
+      <c r="G596" s="13"/>
     </row>
     <row r="597">
-      <c r="G597" s="16"/>
+      <c r="G597" s="13"/>
     </row>
     <row r="598">
-      <c r="G598" s="16"/>
+      <c r="G598" s="13"/>
     </row>
     <row r="599">
-      <c r="G599" s="16"/>
+      <c r="G599" s="13"/>
     </row>
     <row r="600">
-      <c r="G600" s="16"/>
+      <c r="G600" s="13"/>
     </row>
     <row r="601">
-      <c r="G601" s="16"/>
+      <c r="G601" s="13"/>
     </row>
     <row r="602">
-      <c r="G602" s="16"/>
+      <c r="G602" s="13"/>
     </row>
     <row r="603">
-      <c r="G603" s="16"/>
+      <c r="G603" s="13"/>
     </row>
     <row r="604">
-      <c r="G604" s="16"/>
+      <c r="G604" s="13"/>
     </row>
     <row r="605">
-      <c r="G605" s="16"/>
+      <c r="G605" s="13"/>
     </row>
     <row r="606">
-      <c r="G606" s="16"/>
+      <c r="G606" s="13"/>
     </row>
     <row r="607">
-      <c r="G607" s="16"/>
+      <c r="G607" s="13"/>
     </row>
     <row r="608">
-      <c r="G608" s="16"/>
+      <c r="G608" s="13"/>
     </row>
     <row r="609">
-      <c r="G609" s="16"/>
+      <c r="G609" s="13"/>
     </row>
     <row r="610">
-      <c r="G610" s="16"/>
+      <c r="G610" s="13"/>
     </row>
     <row r="611">
-      <c r="G611" s="16"/>
+      <c r="G611" s="13"/>
     </row>
     <row r="612">
-      <c r="G612" s="16"/>
+      <c r="G612" s="13"/>
     </row>
     <row r="613">
-      <c r="G613" s="16"/>
+      <c r="G613" s="13"/>
     </row>
     <row r="614">
-      <c r="G614" s="16"/>
+      <c r="G614" s="13"/>
     </row>
     <row r="615">
-      <c r="G615" s="16"/>
+      <c r="G615" s="13"/>
     </row>
     <row r="616">
-      <c r="G616" s="16"/>
+      <c r="G616" s="13"/>
     </row>
     <row r="617">
-      <c r="G617" s="16"/>
+      <c r="G617" s="13"/>
     </row>
     <row r="618">
-      <c r="G618" s="16"/>
+      <c r="G618" s="13"/>
     </row>
     <row r="619">
-      <c r="G619" s="16"/>
+      <c r="G619" s="13"/>
     </row>
     <row r="620">
-      <c r="G620" s="16"/>
+      <c r="G620" s="13"/>
     </row>
     <row r="621">
-      <c r="G621" s="16"/>
+      <c r="G621" s="13"/>
     </row>
     <row r="622">
-      <c r="G622" s="16"/>
+      <c r="G622" s="13"/>
     </row>
     <row r="623">
-      <c r="G623" s="16"/>
+      <c r="G623" s="13"/>
     </row>
     <row r="624">
-      <c r="G624" s="16"/>
+      <c r="G624" s="13"/>
     </row>
     <row r="625">
-      <c r="G625" s="16"/>
+      <c r="G625" s="13"/>
     </row>
     <row r="626">
-      <c r="G626" s="16"/>
+      <c r="G626" s="13"/>
     </row>
     <row r="627">
-      <c r="G627" s="16"/>
+      <c r="G627" s="13"/>
     </row>
     <row r="628">
-      <c r="G628" s="16"/>
+      <c r="G628" s="13"/>
     </row>
     <row r="629">
-      <c r="G629" s="16"/>
+      <c r="G629" s="13"/>
     </row>
     <row r="630">
-      <c r="G630" s="16"/>
+      <c r="G630" s="13"/>
     </row>
     <row r="631">
-      <c r="G631" s="16"/>
+      <c r="G631" s="13"/>
     </row>
     <row r="632">
-      <c r="G632" s="16"/>
+      <c r="G632" s="13"/>
     </row>
     <row r="633">
-      <c r="G633" s="16"/>
+      <c r="G633" s="13"/>
     </row>
     <row r="634">
-      <c r="G634" s="16"/>
+      <c r="G634" s="13"/>
     </row>
     <row r="635">
-      <c r="G635" s="16"/>
+      <c r="G635" s="13"/>
     </row>
     <row r="636">
-      <c r="G636" s="16"/>
+      <c r="G636" s="13"/>
     </row>
     <row r="637">
-      <c r="G637" s="16"/>
+      <c r="G637" s="13"/>
     </row>
     <row r="638">
-      <c r="G638" s="16"/>
+      <c r="G638" s="13"/>
     </row>
     <row r="639">
-      <c r="G639" s="16"/>
+      <c r="G639" s="13"/>
     </row>
     <row r="640">
-      <c r="G640" s="16"/>
+      <c r="G640" s="13"/>
     </row>
     <row r="641">
-      <c r="G641" s="16"/>
+      <c r="G641" s="13"/>
     </row>
     <row r="642">
-      <c r="G642" s="16"/>
+      <c r="G642" s="13"/>
     </row>
     <row r="643">
-      <c r="G643" s="16"/>
+      <c r="G643" s="13"/>
     </row>
     <row r="644">
-      <c r="G644" s="16"/>
+      <c r="G644" s="13"/>
     </row>
     <row r="645">
-      <c r="G645" s="16"/>
+      <c r="G645" s="13"/>
     </row>
     <row r="646">
-      <c r="G646" s="16"/>
+      <c r="G646" s="13"/>
     </row>
     <row r="647">
-      <c r="G647" s="16"/>
+      <c r="G647" s="13"/>
     </row>
     <row r="648">
-      <c r="G648" s="16"/>
+      <c r="G648" s="13"/>
     </row>
     <row r="649">
-      <c r="G649" s="16"/>
+      <c r="G649" s="13"/>
     </row>
     <row r="650">
-      <c r="G650" s="16"/>
+      <c r="G650" s="13"/>
     </row>
     <row r="651">
-      <c r="G651" s="16"/>
+      <c r="G651" s="13"/>
     </row>
     <row r="652">
-      <c r="G652" s="16"/>
+      <c r="G652" s="13"/>
     </row>
     <row r="653">
-      <c r="G653" s="16"/>
+      <c r="G653" s="13"/>
     </row>
     <row r="654">
-      <c r="G654" s="16"/>
+      <c r="G654" s="13"/>
     </row>
     <row r="655">
-      <c r="G655" s="16"/>
+      <c r="G655" s="13"/>
     </row>
     <row r="656">
-      <c r="G656" s="16"/>
+      <c r="G656" s="13"/>
     </row>
     <row r="657">
-      <c r="G657" s="16"/>
+      <c r="G657" s="13"/>
     </row>
     <row r="658">
-      <c r="G658" s="16"/>
+      <c r="G658" s="13"/>
     </row>
     <row r="659">
-      <c r="G659" s="16"/>
+      <c r="G659" s="13"/>
     </row>
     <row r="660">
-      <c r="G660" s="16"/>
+      <c r="G660" s="13"/>
     </row>
     <row r="661">
-      <c r="G661" s="16"/>
+      <c r="G661" s="13"/>
     </row>
     <row r="662">
-      <c r="G662" s="16"/>
+      <c r="G662" s="13"/>
     </row>
     <row r="663">
-      <c r="G663" s="16"/>
+      <c r="G663" s="13"/>
     </row>
     <row r="664">
-      <c r="G664" s="16"/>
+      <c r="G664" s="13"/>
     </row>
     <row r="665">
-      <c r="G665" s="16"/>
+      <c r="G665" s="13"/>
     </row>
     <row r="666">
-      <c r="G666" s="16"/>
+      <c r="G666" s="13"/>
     </row>
     <row r="667">
-      <c r="G667" s="16"/>
+      <c r="G667" s="13"/>
     </row>
     <row r="668">
-      <c r="G668" s="16"/>
+      <c r="G668" s="13"/>
     </row>
     <row r="669">
-      <c r="G669" s="16"/>
+      <c r="G669" s="13"/>
     </row>
     <row r="670">
-      <c r="G670" s="16"/>
+      <c r="G670" s="13"/>
     </row>
     <row r="671">
-      <c r="G671" s="16"/>
+      <c r="G671" s="13"/>
     </row>
     <row r="672">
-      <c r="G672" s="16"/>
+      <c r="G672" s="13"/>
     </row>
     <row r="673">
-      <c r="G673" s="16"/>
+      <c r="G673" s="13"/>
     </row>
     <row r="674">
-      <c r="G674" s="16"/>
+      <c r="G674" s="13"/>
     </row>
     <row r="675">
-      <c r="G675" s="16"/>
+      <c r="G675" s="13"/>
     </row>
     <row r="676">
-      <c r="G676" s="16"/>
+      <c r="G676" s="13"/>
     </row>
     <row r="677">
-      <c r="G677" s="16"/>
+      <c r="G677" s="13"/>
     </row>
     <row r="678">
-      <c r="G678" s="16"/>
+      <c r="G678" s="13"/>
     </row>
     <row r="679">
-      <c r="G679" s="16"/>
+      <c r="G679" s="13"/>
     </row>
     <row r="680">
-      <c r="G680" s="16"/>
+      <c r="G680" s="13"/>
     </row>
     <row r="681">
-      <c r="G681" s="16"/>
+      <c r="G681" s="13"/>
     </row>
     <row r="682">
-      <c r="G682" s="16"/>
+      <c r="G682" s="13"/>
     </row>
     <row r="683">
-      <c r="G683" s="16"/>
+      <c r="G683" s="13"/>
     </row>
     <row r="684">
-      <c r="G684" s="16"/>
+      <c r="G684" s="13"/>
     </row>
     <row r="685">
-      <c r="G685" s="16"/>
+      <c r="G685" s="13"/>
     </row>
     <row r="686">
-      <c r="G686" s="16"/>
+      <c r="G686" s="13"/>
     </row>
     <row r="687">
-      <c r="G687" s="16"/>
+      <c r="G687" s="13"/>
     </row>
     <row r="688">
-      <c r="G688" s="16"/>
+      <c r="G688" s="13"/>
     </row>
     <row r="689">
-      <c r="G689" s="16"/>
+      <c r="G689" s="13"/>
     </row>
     <row r="690">
-      <c r="G690" s="16"/>
+      <c r="G690" s="13"/>
     </row>
     <row r="691">
-      <c r="G691" s="16"/>
+      <c r="G691" s="13"/>
     </row>
     <row r="692">
-      <c r="G692" s="16"/>
+      <c r="G692" s="13"/>
     </row>
     <row r="693">
-      <c r="G693" s="16"/>
+      <c r="G693" s="13"/>
     </row>
     <row r="694">
-      <c r="G694" s="16"/>
+      <c r="G694" s="13"/>
     </row>
     <row r="695">
-      <c r="G695" s="16"/>
+      <c r="G695" s="13"/>
     </row>
     <row r="696">
-      <c r="G696" s="16"/>
+      <c r="G696" s="13"/>
     </row>
     <row r="697">
-      <c r="G697" s="16"/>
+      <c r="G697" s="13"/>
     </row>
     <row r="698">
-      <c r="G698" s="16"/>
+      <c r="G698" s="13"/>
     </row>
     <row r="699">
-      <c r="G699" s="16"/>
+      <c r="G699" s="13"/>
     </row>
     <row r="700">
-      <c r="G700" s="16"/>
+      <c r="G700" s="13"/>
     </row>
     <row r="701">
-      <c r="G701" s="16"/>
+      <c r="G701" s="13"/>
     </row>
     <row r="702">
-      <c r="G702" s="16"/>
+      <c r="G702" s="13"/>
     </row>
     <row r="703">
-      <c r="G703" s="16"/>
+      <c r="G703" s="13"/>
     </row>
     <row r="704">
-      <c r="G704" s="16"/>
+      <c r="G704" s="13"/>
     </row>
     <row r="705">
-      <c r="G705" s="16"/>
+      <c r="G705" s="13"/>
     </row>
     <row r="706">
-      <c r="G706" s="16"/>
+      <c r="G706" s="13"/>
     </row>
     <row r="707">
-      <c r="G707" s="16"/>
+      <c r="G707" s="13"/>
     </row>
     <row r="708">
-      <c r="G708" s="16"/>
+      <c r="G708" s="13"/>
     </row>
     <row r="709">
-      <c r="G709" s="16"/>
+      <c r="G709" s="13"/>
     </row>
     <row r="710">
-      <c r="G710" s="16"/>
+      <c r="G710" s="13"/>
     </row>
     <row r="711">
-      <c r="G711" s="16"/>
+      <c r="G711" s="13"/>
     </row>
     <row r="712">
-      <c r="G712" s="16"/>
+      <c r="G712" s="13"/>
     </row>
     <row r="713">
-      <c r="G713" s="16"/>
+      <c r="G713" s="13"/>
     </row>
     <row r="714">
-      <c r="G714" s="16"/>
+      <c r="G714" s="13"/>
     </row>
     <row r="715">
-      <c r="G715" s="16"/>
+      <c r="G715" s="13"/>
     </row>
     <row r="716">
-      <c r="G716" s="16"/>
+      <c r="G716" s="13"/>
     </row>
     <row r="717">
-      <c r="G717" s="16"/>
+      <c r="G717" s="13"/>
     </row>
     <row r="718">
-      <c r="G718" s="16"/>
+      <c r="G718" s="13"/>
     </row>
     <row r="719">
-      <c r="G719" s="16"/>
+      <c r="G719" s="13"/>
     </row>
     <row r="720">
-      <c r="G720" s="16"/>
+      <c r="G720" s="13"/>
     </row>
     <row r="721">
-      <c r="G721" s="16"/>
+      <c r="G721" s="13"/>
     </row>
     <row r="722">
-      <c r="G722" s="16"/>
+      <c r="G722" s="13"/>
     </row>
     <row r="723">
-      <c r="G723" s="16"/>
+      <c r="G723" s="13"/>
     </row>
     <row r="724">
-      <c r="G724" s="16"/>
+      <c r="G724" s="13"/>
     </row>
     <row r="725">
-      <c r="G725" s="16"/>
+      <c r="G725" s="13"/>
     </row>
     <row r="726">
-      <c r="G726" s="16"/>
+      <c r="G726" s="13"/>
     </row>
     <row r="727">
-      <c r="G727" s="16"/>
+      <c r="G727" s="13"/>
     </row>
     <row r="728">
-      <c r="G728" s="16"/>
+      <c r="G728" s="13"/>
     </row>
     <row r="729">
-      <c r="G729" s="16"/>
+      <c r="G729" s="13"/>
     </row>
     <row r="730">
-      <c r="G730" s="16"/>
+      <c r="G730" s="13"/>
     </row>
     <row r="731">
-      <c r="G731" s="16"/>
+      <c r="G731" s="13"/>
     </row>
     <row r="732">
-      <c r="G732" s="16"/>
+      <c r="G732" s="13"/>
     </row>
     <row r="733">
-      <c r="G733" s="16"/>
+      <c r="G733" s="13"/>
     </row>
     <row r="734">
-      <c r="G734" s="16"/>
+      <c r="G734" s="13"/>
     </row>
     <row r="735">
-      <c r="G735" s="16"/>
+      <c r="G735" s="13"/>
     </row>
     <row r="736">
-      <c r="G736" s="16"/>
+      <c r="G736" s="13"/>
     </row>
     <row r="737">
-      <c r="G737" s="16"/>
+      <c r="G737" s="13"/>
     </row>
     <row r="738">
-      <c r="G738" s="16"/>
+      <c r="G738" s="13"/>
     </row>
     <row r="739">
-      <c r="G739" s="16"/>
+      <c r="G739" s="13"/>
     </row>
     <row r="740">
-      <c r="G740" s="16"/>
+      <c r="G740" s="13"/>
     </row>
     <row r="741">
-      <c r="G741" s="16"/>
+      <c r="G741" s="13"/>
     </row>
     <row r="742">
-      <c r="G742" s="16"/>
+      <c r="G742" s="13"/>
     </row>
     <row r="743">
-      <c r="G743" s="16"/>
+      <c r="G743" s="13"/>
     </row>
     <row r="744">
-      <c r="G744" s="16"/>
+      <c r="G744" s="13"/>
     </row>
     <row r="745">
-      <c r="G745" s="16"/>
+      <c r="G745" s="13"/>
     </row>
     <row r="746">
-      <c r="G746" s="16"/>
+      <c r="G746" s="13"/>
     </row>
     <row r="747">
-      <c r="G747" s="16"/>
+      <c r="G747" s="13"/>
     </row>
     <row r="748">
-      <c r="G748" s="16"/>
+      <c r="G748" s="13"/>
     </row>
     <row r="749">
-      <c r="G749" s="16"/>
+      <c r="G749" s="13"/>
     </row>
     <row r="750">
-      <c r="G750" s="16"/>
+      <c r="G750" s="13"/>
     </row>
     <row r="751">
-      <c r="G751" s="16"/>
+      <c r="G751" s="13"/>
     </row>
     <row r="752">
-      <c r="G752" s="16"/>
+      <c r="G752" s="13"/>
     </row>
     <row r="753">
-      <c r="G753" s="16"/>
+      <c r="G753" s="13"/>
     </row>
     <row r="754">
-      <c r="G754" s="16"/>
+      <c r="G754" s="13"/>
     </row>
     <row r="755">
-      <c r="G755" s="16"/>
+      <c r="G755" s="13"/>
     </row>
     <row r="756">
-      <c r="G756" s="16"/>
+      <c r="G756" s="13"/>
     </row>
     <row r="757">
-      <c r="G757" s="16"/>
+      <c r="G757" s="13"/>
     </row>
     <row r="758">
-      <c r="G758" s="16"/>
+      <c r="G758" s="13"/>
     </row>
     <row r="759">
-      <c r="G759" s="16"/>
+      <c r="G759" s="13"/>
     </row>
     <row r="760">
-      <c r="G760" s="16"/>
+      <c r="G760" s="13"/>
     </row>
     <row r="761">
-      <c r="G761" s="16"/>
+      <c r="G761" s="13"/>
     </row>
     <row r="762">
-      <c r="G762" s="16"/>
+      <c r="G762" s="13"/>
     </row>
     <row r="763">
-      <c r="G763" s="16"/>
+      <c r="G763" s="13"/>
     </row>
     <row r="764">
-      <c r="G764" s="16"/>
+      <c r="G764" s="13"/>
     </row>
     <row r="765">
-      <c r="G765" s="16"/>
+      <c r="G765" s="13"/>
     </row>
     <row r="766">
-      <c r="G766" s="16"/>
+      <c r="G766" s="13"/>
     </row>
     <row r="767">
-      <c r="G767" s="16"/>
+      <c r="G767" s="13"/>
     </row>
     <row r="768">
-      <c r="G768" s="16"/>
+      <c r="G768" s="13"/>
     </row>
     <row r="769">
-      <c r="G769" s="16"/>
+      <c r="G769" s="13"/>
     </row>
     <row r="770">
-      <c r="G770" s="16"/>
+      <c r="G770" s="13"/>
     </row>
     <row r="771">
-      <c r="G771" s="16"/>
+      <c r="G771" s="13"/>
     </row>
     <row r="772">
-      <c r="G772" s="16"/>
+      <c r="G772" s="13"/>
     </row>
     <row r="773">
-      <c r="G773" s="16"/>
+      <c r="G773" s="13"/>
     </row>
     <row r="774">
-      <c r="G774" s="16"/>
+      <c r="G774" s="13"/>
     </row>
     <row r="775">
-      <c r="G775" s="16"/>
+      <c r="G775" s="13"/>
     </row>
     <row r="776">
-      <c r="G776" s="16"/>
+      <c r="G776" s="13"/>
     </row>
     <row r="777">
-      <c r="G777" s="16"/>
+      <c r="G777" s="13"/>
     </row>
     <row r="778">
-      <c r="G778" s="16"/>
+      <c r="G778" s="13"/>
     </row>
     <row r="779">
-      <c r="G779" s="16"/>
+      <c r="G779" s="13"/>
     </row>
     <row r="780">
-      <c r="G780" s="16"/>
+      <c r="G780" s="13"/>
     </row>
     <row r="781">
-      <c r="G781" s="16"/>
+      <c r="G781" s="13"/>
     </row>
     <row r="782">
-      <c r="G782" s="16"/>
+      <c r="G782" s="13"/>
     </row>
     <row r="783">
-      <c r="G783" s="16"/>
+      <c r="G783" s="13"/>
     </row>
     <row r="784">
-      <c r="G784" s="16"/>
+      <c r="G784" s="13"/>
     </row>
     <row r="785">
-      <c r="G785" s="16"/>
+      <c r="G785" s="13"/>
     </row>
     <row r="786">
-      <c r="G786" s="16"/>
+      <c r="G786" s="13"/>
     </row>
     <row r="787">
-      <c r="G787" s="16"/>
+      <c r="G787" s="13"/>
     </row>
     <row r="788">
-      <c r="G788" s="16"/>
+      <c r="G788" s="13"/>
     </row>
     <row r="789">
-      <c r="G789" s="16"/>
+      <c r="G789" s="13"/>
     </row>
     <row r="790">
-      <c r="G790" s="16"/>
+      <c r="G790" s="13"/>
     </row>
     <row r="791">
-      <c r="G791" s="16"/>
+      <c r="G791" s="13"/>
     </row>
     <row r="792">
-      <c r="G792" s="16"/>
+      <c r="G792" s="13"/>
     </row>
     <row r="793">
-      <c r="G793" s="16"/>
+      <c r="G793" s="13"/>
     </row>
     <row r="794">
-      <c r="G794" s="16"/>
+      <c r="G794" s="13"/>
     </row>
     <row r="795">
-      <c r="G795" s="16"/>
+      <c r="G795" s="13"/>
     </row>
     <row r="796">
-      <c r="G796" s="16"/>
+      <c r="G796" s="13"/>
     </row>
     <row r="797">
-      <c r="G797" s="16"/>
+      <c r="G797" s="13"/>
     </row>
     <row r="798">
-      <c r="G798" s="16"/>
+      <c r="G798" s="13"/>
     </row>
     <row r="799">
-      <c r="G799" s="16"/>
+      <c r="G799" s="13"/>
     </row>
     <row r="800">
-      <c r="G800" s="16"/>
+      <c r="G800" s="13"/>
     </row>
     <row r="801">
-      <c r="G801" s="16"/>
+      <c r="G801" s="13"/>
     </row>
     <row r="802">
-      <c r="G802" s="16"/>
+      <c r="G802" s="13"/>
     </row>
     <row r="803">
-      <c r="G803" s="16"/>
+      <c r="G803" s="13"/>
     </row>
     <row r="804">
-      <c r="G804" s="16"/>
+      <c r="G804" s="13"/>
     </row>
     <row r="805">
-      <c r="G805" s="16"/>
+      <c r="G805" s="13"/>
     </row>
     <row r="806">
-      <c r="G806" s="16"/>
+      <c r="G806" s="13"/>
     </row>
     <row r="807">
-      <c r="G807" s="16"/>
+      <c r="G807" s="13"/>
     </row>
     <row r="808">
-      <c r="G808" s="16"/>
+      <c r="G808" s="13"/>
     </row>
     <row r="809">
-      <c r="G809" s="16"/>
+      <c r="G809" s="13"/>
     </row>
     <row r="810">
-      <c r="G810" s="16"/>
+      <c r="G810" s="13"/>
     </row>
     <row r="811">
-      <c r="G811" s="16"/>
+      <c r="G811" s="13"/>
     </row>
     <row r="812">
-      <c r="G812" s="16"/>
+      <c r="G812" s="13"/>
     </row>
     <row r="813">
-      <c r="G813" s="16"/>
+      <c r="G813" s="13"/>
     </row>
     <row r="814">
-      <c r="G814" s="16"/>
+      <c r="G814" s="13"/>
     </row>
     <row r="815">
-      <c r="G815" s="16"/>
+      <c r="G815" s="13"/>
     </row>
     <row r="816">
-      <c r="G816" s="16"/>
+      <c r="G816" s="13"/>
     </row>
     <row r="817">
-      <c r="G817" s="16"/>
+      <c r="G817" s="13"/>
     </row>
     <row r="818">
-      <c r="G818" s="16"/>
+      <c r="G818" s="13"/>
     </row>
     <row r="819">
-      <c r="G819" s="16"/>
+      <c r="G819" s="13"/>
     </row>
     <row r="820">
-      <c r="G820" s="16"/>
+      <c r="G820" s="13"/>
     </row>
     <row r="821">
-      <c r="G821" s="16"/>
+      <c r="G821" s="13"/>
     </row>
     <row r="822">
-      <c r="G822" s="16"/>
+      <c r="G822" s="13"/>
     </row>
     <row r="823">
-      <c r="G823" s="16"/>
+      <c r="G823" s="13"/>
     </row>
     <row r="824">
-      <c r="G824" s="16"/>
+      <c r="G824" s="13"/>
     </row>
     <row r="825">
-      <c r="G825" s="16"/>
+      <c r="G825" s="13"/>
     </row>
     <row r="826">
-      <c r="G826" s="16"/>
+      <c r="G826" s="13"/>
     </row>
     <row r="827">
-      <c r="G827" s="16"/>
+      <c r="G827" s="13"/>
     </row>
     <row r="828">
-      <c r="G828" s="16"/>
+      <c r="G828" s="13"/>
     </row>
     <row r="829">
-      <c r="G829" s="16"/>
+      <c r="G829" s="13"/>
     </row>
     <row r="830">
-      <c r="G830" s="16"/>
+      <c r="G830" s="13"/>
     </row>
     <row r="831">
-      <c r="G831" s="16"/>
+      <c r="G831" s="13"/>
     </row>
     <row r="832">
-      <c r="G832" s="16"/>
+      <c r="G832" s="13"/>
     </row>
     <row r="833">
-      <c r="G833" s="16"/>
+      <c r="G833" s="13"/>
     </row>
     <row r="834">
-      <c r="G834" s="16"/>
+      <c r="G834" s="13"/>
     </row>
     <row r="835">
-      <c r="G835" s="16"/>
+      <c r="G835" s="13"/>
     </row>
     <row r="836">
-      <c r="G836" s="16"/>
+      <c r="G836" s="13"/>
     </row>
     <row r="837">
-      <c r="G837" s="16"/>
+      <c r="G837" s="13"/>
     </row>
     <row r="838">
-      <c r="G838" s="16"/>
+      <c r="G838" s="13"/>
     </row>
     <row r="839">
-      <c r="G839" s="16"/>
+      <c r="G839" s="13"/>
     </row>
     <row r="840">
-      <c r="G840" s="16"/>
+      <c r="G840" s="13"/>
     </row>
     <row r="841">
-      <c r="G841" s="16"/>
+      <c r="G841" s="13"/>
     </row>
     <row r="842">
-      <c r="G842" s="16"/>
+      <c r="G842" s="13"/>
     </row>
     <row r="843">
-      <c r="G843" s="16"/>
+      <c r="G843" s="13"/>
     </row>
     <row r="844">
-      <c r="G844" s="16"/>
+      <c r="G844" s="13"/>
     </row>
     <row r="845">
-      <c r="G845" s="16"/>
+      <c r="G845" s="13"/>
     </row>
     <row r="846">
-      <c r="G846" s="16"/>
+      <c r="G846" s="13"/>
     </row>
     <row r="847">
-      <c r="G847" s="16"/>
+      <c r="G847" s="13"/>
     </row>
     <row r="848">
-      <c r="G848" s="16"/>
+      <c r="G848" s="13"/>
     </row>
     <row r="849">
-      <c r="G849" s="16"/>
+      <c r="G849" s="13"/>
     </row>
     <row r="850">
-      <c r="G850" s="16"/>
+      <c r="G850" s="13"/>
     </row>
     <row r="851">
-      <c r="G851" s="16"/>
+      <c r="G851" s="13"/>
     </row>
     <row r="852">
-      <c r="G852" s="16"/>
+      <c r="G852" s="13"/>
     </row>
     <row r="853">
-      <c r="G853" s="16"/>
+      <c r="G853" s="13"/>
     </row>
     <row r="854">
-      <c r="G854" s="16"/>
+      <c r="G854" s="13"/>
     </row>
     <row r="855">
-      <c r="G855" s="16"/>
+      <c r="G855" s="13"/>
     </row>
     <row r="856">
-      <c r="G856" s="16"/>
+      <c r="G856" s="13"/>
     </row>
     <row r="857">
-      <c r="G857" s="16"/>
+      <c r="G857" s="13"/>
     </row>
     <row r="858">
-      <c r="G858" s="16"/>
+      <c r="G858" s="13"/>
     </row>
     <row r="859">
-      <c r="G859" s="16"/>
+      <c r="G859" s="13"/>
     </row>
     <row r="860">
-      <c r="G860" s="16"/>
+      <c r="G860" s="13"/>
     </row>
     <row r="861">
-      <c r="G861" s="16"/>
+      <c r="G861" s="13"/>
     </row>
     <row r="862">
-      <c r="G862" s="16"/>
+      <c r="G862" s="13"/>
     </row>
     <row r="863">
-      <c r="G863" s="16"/>
+      <c r="G863" s="13"/>
     </row>
     <row r="864">
-      <c r="G864" s="16"/>
+      <c r="G864" s="13"/>
     </row>
     <row r="865">
-      <c r="G865" s="16"/>
+      <c r="G865" s="13"/>
     </row>
     <row r="866">
-      <c r="G866" s="16"/>
+      <c r="G866" s="13"/>
     </row>
     <row r="867">
-      <c r="G867" s="16"/>
+      <c r="G867" s="13"/>
     </row>
     <row r="868">
-      <c r="G868" s="16"/>
+      <c r="G868" s="13"/>
     </row>
     <row r="869">
-      <c r="G869" s="16"/>
+      <c r="G869" s="13"/>
     </row>
     <row r="870">
-      <c r="G870" s="16"/>
+      <c r="G870" s="13"/>
     </row>
     <row r="871">
-      <c r="G871" s="16"/>
+      <c r="G871" s="13"/>
     </row>
     <row r="872">
-      <c r="G872" s="16"/>
+      <c r="G872" s="13"/>
     </row>
     <row r="873">
-      <c r="G873" s="16"/>
+      <c r="G873" s="13"/>
     </row>
     <row r="874">
-      <c r="G874" s="16"/>
+      <c r="G874" s="13"/>
     </row>
     <row r="875">
-      <c r="G875" s="16"/>
+      <c r="G875" s="13"/>
     </row>
     <row r="876">
-      <c r="G876" s="16"/>
+      <c r="G876" s="13"/>
     </row>
     <row r="877">
-      <c r="G877" s="16"/>
+      <c r="G877" s="13"/>
     </row>
     <row r="878">
-      <c r="G878" s="16"/>
+      <c r="G878" s="13"/>
     </row>
     <row r="879">
-      <c r="G879" s="16"/>
+      <c r="G879" s="13"/>
     </row>
     <row r="880">
-      <c r="G880" s="16"/>
+      <c r="G880" s="13"/>
     </row>
     <row r="881">
-      <c r="G881" s="16"/>
+      <c r="G881" s="13"/>
     </row>
     <row r="882">
-      <c r="G882" s="16"/>
+      <c r="G882" s="13"/>
     </row>
     <row r="883">
-      <c r="G883" s="16"/>
+      <c r="G883" s="13"/>
     </row>
     <row r="884">
-      <c r="G884" s="16"/>
+      <c r="G884" s="13"/>
     </row>
     <row r="885">
-      <c r="G885" s="16"/>
+      <c r="G885" s="13"/>
     </row>
     <row r="886">
-      <c r="G886" s="16"/>
+      <c r="G886" s="13"/>
     </row>
     <row r="887">
-      <c r="G887" s="16"/>
+      <c r="G887" s="13"/>
     </row>
     <row r="888">
-      <c r="G888" s="16"/>
+      <c r="G888" s="13"/>
     </row>
     <row r="889">
-      <c r="G889" s="16"/>
+      <c r="G889" s="13"/>
     </row>
     <row r="890">
-      <c r="G890" s="16"/>
+      <c r="G890" s="13"/>
     </row>
     <row r="891">
-      <c r="G891" s="16"/>
+      <c r="G891" s="13"/>
     </row>
     <row r="892">
-      <c r="G892" s="16"/>
+      <c r="G892" s="13"/>
     </row>
     <row r="893">
-      <c r="G893" s="16"/>
+      <c r="G893" s="13"/>
     </row>
     <row r="894">
-      <c r="G894" s="16"/>
+      <c r="G894" s="13"/>
     </row>
     <row r="895">
-      <c r="G895" s="16"/>
+      <c r="G895" s="13"/>
     </row>
     <row r="896">
-      <c r="G896" s="16"/>
+      <c r="G896" s="13"/>
     </row>
     <row r="897">
-      <c r="G897" s="16"/>
+      <c r="G897" s="13"/>
     </row>
     <row r="898">
-      <c r="G898" s="16"/>
+      <c r="G898" s="13"/>
     </row>
     <row r="899">
-      <c r="G899" s="16"/>
+      <c r="G899" s="13"/>
     </row>
     <row r="900">
-      <c r="G900" s="16"/>
+      <c r="G900" s="13"/>
     </row>
     <row r="901">
-      <c r="G901" s="16"/>
+      <c r="G901" s="13"/>
     </row>
     <row r="902">
-      <c r="G902" s="16"/>
+      <c r="G902" s="13"/>
     </row>
     <row r="903">
-      <c r="G903" s="16"/>
+      <c r="G903" s="13"/>
     </row>
     <row r="904">
-      <c r="G904" s="16"/>
+      <c r="G904" s="13"/>
     </row>
     <row r="905">
-      <c r="G905" s="16"/>
+      <c r="G905" s="13"/>
     </row>
     <row r="906">
-      <c r="G906" s="16"/>
+      <c r="G906" s="13"/>
     </row>
     <row r="907">
-      <c r="G907" s="16"/>
+      <c r="G907" s="13"/>
     </row>
     <row r="908">
-      <c r="G908" s="16"/>
+      <c r="G908" s="13"/>
     </row>
     <row r="909">
-      <c r="G909" s="16"/>
+      <c r="G909" s="13"/>
     </row>
     <row r="910">
-      <c r="G910" s="16"/>
+      <c r="G910" s="13"/>
     </row>
     <row r="911">
-      <c r="G911" s="16"/>
+      <c r="G911" s="13"/>
     </row>
     <row r="912">
-      <c r="G912" s="16"/>
+      <c r="G912" s="13"/>
     </row>
     <row r="913">
-      <c r="G913" s="16"/>
+      <c r="G913" s="13"/>
     </row>
     <row r="914">
-      <c r="G914" s="16"/>
+      <c r="G914" s="13"/>
     </row>
     <row r="915">
-      <c r="G915" s="16"/>
+      <c r="G915" s="13"/>
     </row>
     <row r="916">
-      <c r="G916" s="16"/>
+      <c r="G916" s="13"/>
     </row>
     <row r="917">
-      <c r="G917" s="16"/>
+      <c r="G917" s="13"/>
     </row>
     <row r="918">
-      <c r="G918" s="16"/>
+      <c r="G918" s="13"/>
     </row>
     <row r="919">
-      <c r="G919" s="16"/>
+      <c r="G919" s="13"/>
     </row>
     <row r="920">
-      <c r="G920" s="16"/>
+      <c r="G920" s="13"/>
     </row>
     <row r="921">
-      <c r="G921" s="16"/>
+      <c r="G921" s="13"/>
     </row>
     <row r="922">
-      <c r="G922" s="16"/>
+      <c r="G922" s="13"/>
     </row>
     <row r="923">
-      <c r="G923" s="16"/>
+      <c r="G923" s="13"/>
     </row>
     <row r="924">
-      <c r="G924" s="16"/>
+      <c r="G924" s="13"/>
     </row>
     <row r="925">
-      <c r="G925" s="16"/>
+      <c r="G925" s="13"/>
     </row>
     <row r="926">
-      <c r="G926" s="16"/>
+      <c r="G926" s="13"/>
     </row>
     <row r="927">
-      <c r="G927" s="16"/>
+      <c r="G927" s="13"/>
     </row>
     <row r="928">
-      <c r="G928" s="16"/>
+      <c r="G928" s="13"/>
     </row>
     <row r="929">
-      <c r="G929" s="16"/>
+      <c r="G929" s="13"/>
     </row>
     <row r="930">
-      <c r="G930" s="16"/>
+      <c r="G930" s="13"/>
     </row>
     <row r="931">
-      <c r="G931" s="16"/>
+      <c r="G931" s="13"/>
     </row>
     <row r="932">
-      <c r="G932" s="16"/>
+      <c r="G932" s="13"/>
     </row>
     <row r="933">
-      <c r="G933" s="16"/>
+      <c r="G933" s="13"/>
     </row>
     <row r="934">
-      <c r="G934" s="16"/>
+      <c r="G934" s="13"/>
     </row>
     <row r="935">
-      <c r="G935" s="16"/>
+      <c r="G935" s="13"/>
     </row>
     <row r="936">
-      <c r="G936" s="16"/>
+      <c r="G936" s="13"/>
     </row>
     <row r="937">
-      <c r="G937" s="16"/>
+      <c r="G937" s="13"/>
     </row>
     <row r="938">
-      <c r="G938" s="16"/>
+      <c r="G938" s="13"/>
     </row>
     <row r="939">
-      <c r="G939" s="16"/>
+      <c r="G939" s="13"/>
     </row>
     <row r="940">
-      <c r="G940" s="16"/>
+      <c r="G940" s="13"/>
     </row>
     <row r="941">
-      <c r="G941" s="16"/>
+      <c r="G941" s="13"/>
     </row>
     <row r="942">
-      <c r="G942" s="16"/>
+      <c r="G942" s="13"/>
     </row>
     <row r="943">
-      <c r="G943" s="16"/>
+      <c r="G943" s="13"/>
     </row>
     <row r="944">
-      <c r="G944" s="16"/>
+      <c r="G944" s="13"/>
     </row>
     <row r="945">
-      <c r="G945" s="16"/>
+      <c r="G945" s="13"/>
     </row>
     <row r="946">
-      <c r="G946" s="16"/>
+      <c r="G946" s="13"/>
     </row>
     <row r="947">
-      <c r="G947" s="16"/>
+      <c r="G947" s="13"/>
     </row>
     <row r="948">
-      <c r="G948" s="16"/>
+      <c r="G948" s="13"/>
     </row>
     <row r="949">
-      <c r="G949" s="16"/>
+      <c r="G949" s="13"/>
     </row>
     <row r="950">
-      <c r="G950" s="16"/>
+      <c r="G950" s="13"/>
     </row>
     <row r="951">
-      <c r="G951" s="16"/>
+      <c r="G951" s="13"/>
     </row>
     <row r="952">
-      <c r="G952" s="16"/>
+      <c r="G952" s="13"/>
     </row>
     <row r="953">
-      <c r="G953" s="16"/>
+      <c r="G953" s="13"/>
     </row>
     <row r="954">
-      <c r="G954" s="16"/>
+      <c r="G954" s="13"/>
     </row>
     <row r="955">
-      <c r="G955" s="16"/>
+      <c r="G955" s="13"/>
     </row>
     <row r="956">
-      <c r="G956" s="16"/>
+      <c r="G956" s="13"/>
     </row>
     <row r="957">
-      <c r="G957" s="16"/>
+      <c r="G957" s="13"/>
     </row>
     <row r="958">
-      <c r="G958" s="16"/>
+      <c r="G958" s="13"/>
     </row>
     <row r="959">
-      <c r="G959" s="16"/>
+      <c r="G959" s="13"/>
     </row>
     <row r="960">
-      <c r="G960" s="16"/>
+      <c r="G960" s="13"/>
     </row>
     <row r="961">
-      <c r="G961" s="16"/>
+      <c r="G961" s="13"/>
     </row>
     <row r="962">
-      <c r="G962" s="16"/>
+      <c r="G962" s="13"/>
     </row>
     <row r="963">
-      <c r="G963" s="16"/>
+      <c r="G963" s="13"/>
     </row>
     <row r="964">
-      <c r="G964" s="16"/>
+      <c r="G964" s="13"/>
     </row>
     <row r="965">
-      <c r="G965" s="16"/>
+      <c r="G965" s="13"/>
     </row>
     <row r="966">
-      <c r="G966" s="16"/>
+      <c r="G966" s="13"/>
     </row>
     <row r="967">
-      <c r="G967" s="16"/>
+      <c r="G967" s="13"/>
     </row>
     <row r="968">
-      <c r="G968" s="16"/>
+      <c r="G968" s="13"/>
     </row>
     <row r="969">
-      <c r="G969" s="16"/>
+      <c r="G969" s="13"/>
     </row>
     <row r="970">
-      <c r="G970" s="16"/>
+      <c r="G970" s="13"/>
     </row>
     <row r="971">
-      <c r="G971" s="16"/>
+      <c r="G971" s="13"/>
     </row>
     <row r="972">
-      <c r="G972" s="16"/>
+      <c r="G972" s="13"/>
     </row>
     <row r="973">
-      <c r="G973" s="16"/>
+      <c r="G973" s="13"/>
     </row>
     <row r="974">
-      <c r="G974" s="16"/>
+      <c r="G974" s="13"/>
     </row>
     <row r="975">
-      <c r="G975" s="16"/>
+      <c r="G975" s="13"/>
     </row>
     <row r="976">
-      <c r="G976" s="16"/>
+      <c r="G976" s="13"/>
     </row>
     <row r="977">
-      <c r="G977" s="16"/>
+      <c r="G977" s="13"/>
     </row>
     <row r="978">
-      <c r="G978" s="16"/>
+      <c r="G978" s="13"/>
     </row>
     <row r="979">
-      <c r="G979" s="16"/>
+      <c r="G979" s="13"/>
     </row>
     <row r="980">
-      <c r="G980" s="16"/>
+      <c r="G980" s="13"/>
     </row>
     <row r="981">
-      <c r="G981" s="16"/>
+      <c r="G981" s="13"/>
     </row>
     <row r="982">
-      <c r="G982" s="16"/>
+      <c r="G982" s="13"/>
     </row>
     <row r="983">
-      <c r="G983" s="16"/>
+      <c r="G983" s="13"/>
     </row>
     <row r="984">
-      <c r="G984" s="16"/>
+      <c r="G984" s="13"/>
     </row>
     <row r="985">
-      <c r="G985" s="16"/>
+      <c r="G985" s="13"/>
     </row>
     <row r="986">
-      <c r="G986" s="16"/>
+      <c r="G986" s="13"/>
     </row>
     <row r="987">
-      <c r="G987" s="16"/>
+      <c r="G987" s="13"/>
     </row>
     <row r="988">
-      <c r="G988" s="16"/>
+      <c r="G988" s="13"/>
     </row>
     <row r="989">
-      <c r="G989" s="16"/>
+      <c r="G989" s="13"/>
     </row>
     <row r="990">
-      <c r="G990" s="16"/>
+      <c r="G990" s="13"/>
     </row>
     <row r="991">
-      <c r="G991" s="16"/>
+      <c r="G991" s="13"/>
     </row>
     <row r="992">
-      <c r="G992" s="16"/>
+      <c r="G992" s="13"/>
     </row>
     <row r="993">
-      <c r="G993" s="16"/>
+      <c r="G993" s="13"/>
     </row>
     <row r="994">
-      <c r="G994" s="16"/>
+      <c r="G994" s="13"/>
     </row>
     <row r="995">
-      <c r="G995" s="16"/>
+      <c r="G995" s="13"/>
     </row>
     <row r="996">
-      <c r="G996" s="16"/>
+      <c r="G996" s="13"/>
     </row>
     <row r="997">
-      <c r="G997" s="16"/>
+      <c r="G997" s="13"/>
     </row>
     <row r="998">
-      <c r="G998" s="16"/>
+      <c r="G998" s="13"/>
     </row>
     <row r="999">
-      <c r="G999" s="16"/>
+      <c r="G999" s="13"/>
     </row>
     <row r="1000">
-      <c r="G1000" s="16"/>
+      <c r="G1000" s="13"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="E3"/>
-    <hyperlink r:id="rId1" ref="E4"/>
-    <hyperlink r:id="rId2" ref="E5"/>
-  </hyperlinks>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
-  <extLst>
-    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00370062-00A0-4510-B42B-00F2003B0021}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
-          <x14:formula1>
-            <xm:f>"E Invoice,EWay Bill,GSTR,ITC Reconsilation,LMS,Safe Sign,Third Eye"</xm:f>
-          </x14:formula1>
-          <xm:sqref>G3:G1000</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G3:G1000">
+      <formula1>"E Invoice,EWay Bill,GSTR,ITC Reconsilation,LMS,Safe Sign,Third Eye"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>